<commit_message>
Add logical enclosure with EBIPA
Signed-off-by: Dung K Hoang <DungKHoang@gmail.com>
</commit_message>
<xml_diff>
--- a/Example-Export-OV-sheets.xlsx
+++ b/Example-Export-OV-sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Scripts\Export-Import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github-Temp\Import-Export-OneView-Resources-8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5CC113-2A0B-4AC9-AC29-E96085896147}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871CC967-A659-4261-9A96-D69F3849B431}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="723" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="723" firstSheet="20" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="11" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8241" uniqueCount="1623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8246" uniqueCount="1628">
   <si>
     <t>Pod</t>
   </si>
@@ -6772,6 +6772,52 @@
   </si>
   <si>
     <t>user2-display</t>
+  </si>
+  <si>
+    <t>enclosureNewName</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="5" tint="0.59999389629810485"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"># Manual input: Provide new names for enclosures </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+#Leave empty if you don't want to rename enclosures. 
+# Use '|'as separator</t>
+    </r>
+  </si>
+  <si>
+    <t>manualAddresses</t>
+  </si>
+  <si>
+    <t># EBPIA</t>
+  </si>
+  <si>
+    <t>Frame1=@{Device3={IPv4Address='10.10.4.13'};
+Interconnect6={IPv4Address='10.10.4.16'}}\
+Frame2=@{Device5={IPv4Address='10.10.4.25'};
+Interconnect4={IPv4Address='10.10.4.24'}}\
+Frame3=@{Device8={IPv4Address='10.10.4.38'};
+Interconnect4={IPv4Address='10.10.4.34'}}</t>
   </si>
 </sst>
 </file>
@@ -7133,7 +7179,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -7559,6 +7605,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -10605,7 +10681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
@@ -22684,11 +22760,11 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22696,16 +22772,18 @@
     <col min="1" max="1" width="26.85546875" style="10" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" style="68" customWidth="1"/>
     <col min="3" max="3" width="39" style="10" customWidth="1"/>
-    <col min="4" max="4" width="37" style="10" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" style="152" customWidth="1"/>
+    <col min="4" max="4" width="39" style="166" customWidth="1"/>
+    <col min="5" max="5" width="37" style="10" customWidth="1"/>
+    <col min="6" max="6" width="55.42578125" style="166" customWidth="1"/>
     <col min="7" max="7" width="38.42578125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="49" style="152" customWidth="1"/>
-    <col min="9" max="9" width="45.42578125" style="152" customWidth="1"/>
-    <col min="10" max="10" width="36.140625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="27.85546875" style="152" customWidth="1"/>
+    <col min="9" max="9" width="38.42578125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="49" style="152" customWidth="1"/>
+    <col min="11" max="11" width="45.42578125" style="152" customWidth="1"/>
+    <col min="12" max="12" width="36.140625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -22715,93 +22793,109 @@
       <c r="C1" s="9" t="s">
         <v>872</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="161" t="s">
+        <v>1623</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>873</v>
       </c>
-      <c r="E1" s="153" t="s">
+      <c r="F1" s="161" t="s">
+        <v>1625</v>
+      </c>
+      <c r="G1" s="153" t="s">
         <v>874</v>
       </c>
-      <c r="F1" s="154" t="s">
+      <c r="H1" s="154" t="s">
         <v>875</v>
       </c>
-      <c r="G1" s="153" t="s">
+      <c r="I1" s="153" t="s">
         <v>876</v>
       </c>
-      <c r="H1" s="154" t="s">
+      <c r="J1" s="154" t="s">
         <v>877</v>
       </c>
-      <c r="I1" s="154" t="s">
+      <c r="K1" s="154" t="s">
         <v>878</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="24" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="24" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>879</v>
       </c>
       <c r="B2" s="114"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
+      <c r="D2" s="162"/>
+      <c r="F2" s="162"/>
       <c r="G2" s="129"/>
       <c r="H2" s="129"/>
       <c r="I2" s="129"/>
-    </row>
-    <row r="3" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+    </row>
+    <row r="3" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>880</v>
       </c>
       <c r="B3" s="115"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130"/>
+      <c r="D3" s="163"/>
+      <c r="F3" s="163"/>
       <c r="G3" s="130"/>
       <c r="H3" s="130"/>
       <c r="I3" s="130"/>
-      <c r="J3" s="27"/>
-    </row>
-    <row r="4" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="27"/>
+    </row>
+    <row r="4" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="115"/>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
+      <c r="D4" s="163"/>
+      <c r="F4" s="163"/>
       <c r="G4" s="130"/>
       <c r="H4" s="130"/>
       <c r="I4" s="130"/>
-      <c r="J4" s="23"/>
-    </row>
-    <row r="5" spans="1:13" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J4" s="130"/>
+      <c r="K4" s="130"/>
+      <c r="L4" s="23"/>
+    </row>
+    <row r="5" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>199</v>
       </c>
       <c r="B5" s="115"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
+      <c r="D5" s="163"/>
+      <c r="F5" s="163"/>
       <c r="G5" s="130"/>
       <c r="H5" s="130"/>
       <c r="I5" s="130"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
+      <c r="J5" s="130"/>
+      <c r="K5" s="130"/>
+      <c r="L5" s="23"/>
       <c r="M5" s="27"/>
-    </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+    </row>
+    <row r="6" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
       <c r="B6" s="115"/>
       <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="132"/>
-      <c r="F6" s="133"/>
+      <c r="D6" s="164"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="164"/>
       <c r="G6" s="132"/>
       <c r="H6" s="133"/>
-      <c r="I6" s="133"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="133"/>
+      <c r="K6" s="133"/>
       <c r="M6" s="23"/>
-    </row>
-    <row r="7" spans="1:13" s="47" customFormat="1" ht="193.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+    </row>
+    <row r="7" spans="1:15" s="47" customFormat="1" ht="193.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
         <v>881</v>
       </c>
@@ -22811,88 +22905,104 @@
       <c r="C7" s="46" t="s">
         <v>883</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="165" t="s">
+        <v>1624</v>
+      </c>
+      <c r="E7" s="46" t="s">
         <v>884</v>
       </c>
-      <c r="E7" s="136" t="s">
+      <c r="F7" s="165" t="s">
+        <v>1626</v>
+      </c>
+      <c r="G7" s="136" t="s">
         <v>885</v>
       </c>
-      <c r="F7" s="136" t="s">
+      <c r="H7" s="136" t="s">
         <v>886</v>
       </c>
-      <c r="G7" s="136" t="s">
+      <c r="I7" s="136" t="s">
         <v>887</v>
       </c>
-      <c r="H7" s="136" t="s">
+      <c r="J7" s="136" t="s">
         <v>888</v>
       </c>
-      <c r="I7" s="136" t="s">
+      <c r="K7" s="136" t="s">
         <v>888</v>
       </c>
-      <c r="J7" s="46" t="s">
+      <c r="L7" s="46" t="s">
         <v>339</v>
       </c>
-      <c r="K7" s="48"/>
-      <c r="M7" s="50"/>
-    </row>
-    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="48"/>
+      <c r="O7" s="50"/>
+    </row>
+    <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
       <c r="B8" s="115"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="133"/>
-      <c r="F8" s="133"/>
+      <c r="D8" s="164"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="164"/>
       <c r="G8" s="133"/>
       <c r="H8" s="133"/>
       <c r="I8" s="133"/>
-      <c r="J8" s="23"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J9" s="97"/>
-    </row>
-    <row r="10" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J8" s="133"/>
+      <c r="K8" s="133"/>
+      <c r="L8" s="23"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L9" s="97"/>
+    </row>
+    <row r="10" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="68"/>
       <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="D10" s="167"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="167"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="21"/>
-      <c r="F11" s="15"/>
+      <c r="D11" s="167"/>
       <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="116"/>
       <c r="C12" s="21"/>
-      <c r="D12" s="15"/>
+      <c r="D12" s="167"/>
       <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="F12" s="169"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="21"/>
-    </row>
-    <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="167"/>
+    </row>
+    <row r="14" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="116"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="15"/>
-      <c r="F14" s="152"/>
+      <c r="D14" s="167"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="169"/>
       <c r="H14" s="152"/>
-      <c r="I14" s="152"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J14" s="152"/>
+      <c r="K14" s="152"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:15" ht="180" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>889</v>
       </c>
@@ -22902,51 +23012,64 @@
       <c r="C15" s="21" t="s">
         <v>891</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="167"/>
+      <c r="E15" s="15" t="s">
         <v>868</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="152" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="152" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="170" t="s">
+        <v>1627</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="152" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="152" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="116"/>
       <c r="C16" s="21"/>
-      <c r="D16" s="15"/>
-      <c r="F16" s="152"/>
+      <c r="D16" s="167"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="169"/>
       <c r="H16" s="152"/>
-      <c r="I16" s="152"/>
-      <c r="J16" s="10"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="152"/>
+      <c r="K16" s="152"/>
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C17" s="21"/>
-    </row>
-    <row r="18" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="167"/>
+    </row>
+    <row r="18" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="68"/>
-      <c r="J18" s="10"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D18" s="168"/>
+      <c r="F18" s="168"/>
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C19" s="21"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D19" s="167"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="116"/>
       <c r="C20" s="21"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D20" s="167"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C21" s="21"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D21" s="167"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="116"/>
       <c r="C22" s="21"/>
+      <c r="D22" s="167"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -48270,18 +48393,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -48502,14 +48625,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08671FF-7385-4DFE-A0B1-F772E0CBF546}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43ECCFC7-29C2-4C1C-BA35-7A8B581B0FD8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -48522,6 +48637,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="54a4fa2c-6341-4596-b8d8-a2e023346efc"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08671FF-7385-4DFE-A0B1-F772E0CBF546}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Issue #5 - Custom MAC/WWPN - Boot From SAN
Signed-off-by: Dung K Hoang <DungKHoang@gmail.com>
</commit_message>
<xml_diff>
--- a/Example-Export-OV-sheets.xlsx
+++ b/Example-Export-OV-sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github-Temp\Import-Export-OneView-Resources-8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github-Temp\Import-Export-OneView-Resources-11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871CC967-A659-4261-9A96-D69F3849B431}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1090BA33-F3B2-409D-ADA7-D137985E4274}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="723" firstSheet="20" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="723" firstSheet="29" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="11" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8246" uniqueCount="1628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8152" uniqueCount="1633">
   <si>
     <t>Pod</t>
   </si>
@@ -6155,10 +6155,6 @@
     <t>iqn.2015-02.com.hpe:oneview-vcg3obs0ch</t>
   </si>
   <si>
-    <t>#if userDefined is set to TRUE, we will create a connection with custom MAC and WWN
-# This is a manual configuration. Administrator needs to explicitly set it for the import  operation and apply for server profile only!</t>
-  </si>
-  <si>
     <t>C6:97:ED:90:09:88</t>
   </si>
   <si>
@@ -6818,6 +6814,26 @@
 Interconnect4={IPv4Address='10.10.4.24'}}\
 Frame3=@{Device8={IPv4Address='10.10.4.38'};
 Interconnect4={IPv4Address='10.10.4.34'}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Virtual Connect SE 40Gb F8 Module for Synergy</t>
+  </si>
+  <si>
+    <t>Virtual Connect SE 32Gb FC Module for Synergy</t>
+  </si>
+  <si>
+    <t>bootTarget</t>
+  </si>
+  <si>
+    <t>targetLUN</t>
+  </si>
+  <si>
+    <t># if bootVolumeSource = 'userDefined'
+#Specify WWPN of target LUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># if bootVolumeSource = 'userDefined'
+# Specify lunID of target LUN </t>
   </si>
 </sst>
 </file>
@@ -7179,7 +7195,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -7602,9 +7618,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7635,6 +7648,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="7" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -8662,7 +8691,7 @@
         <v>185</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -8706,7 +8735,7 @@
         <v>187</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -8887,15 +8916,15 @@
       <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D14" s="160"/>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
-      <c r="L14" s="160"/>
+      <c r="D14" s="170"/>
+      <c r="E14" s="170"/>
+      <c r="F14" s="170"/>
+      <c r="G14" s="170"/>
+      <c r="H14" s="170"/>
+      <c r="I14" s="170"/>
+      <c r="J14" s="170"/>
+      <c r="K14" s="170"/>
+      <c r="L14" s="170"/>
     </row>
     <row r="15" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
@@ -9017,7 +9046,7 @@
         <v>190</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="C20" s="63" t="s">
         <v>51</v>
@@ -9040,7 +9069,7 @@
         <v>190</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="C21" s="63" t="s">
         <v>51</v>
@@ -9596,11 +9625,11 @@
       <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
-      <c r="L14" s="160"/>
+      <c r="H14" s="170"/>
+      <c r="I14" s="170"/>
+      <c r="J14" s="170"/>
+      <c r="K14" s="170"/>
+      <c r="L14" s="170"/>
     </row>
     <row r="15" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
@@ -9736,7 +9765,7 @@
         <v>164</v>
       </c>
       <c r="F21" s="63" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="G21" s="63" t="s">
         <v>249</v>
@@ -9759,7 +9788,7 @@
         <v>165</v>
       </c>
       <c r="F22" s="63" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="G22" s="63" t="s">
         <v>245</v>
@@ -15804,9 +15833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:V123"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16056,27 +16085,27 @@
       <c r="M13" s="23"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="D14" s="160"/>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
-      <c r="L14" s="160"/>
-      <c r="M14" s="160"/>
-      <c r="N14" s="160"/>
-      <c r="O14" s="160"/>
-      <c r="P14" s="160"/>
-      <c r="Q14" s="160"/>
-      <c r="R14" s="160"/>
-      <c r="S14" s="160"/>
-      <c r="T14" s="160"/>
-      <c r="U14" s="160"/>
-      <c r="V14" s="160"/>
-    </row>
-    <row r="15" spans="1:22" s="63" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="170"/>
+      <c r="E14" s="170"/>
+      <c r="F14" s="170"/>
+      <c r="G14" s="170"/>
+      <c r="H14" s="170"/>
+      <c r="I14" s="170"/>
+      <c r="J14" s="170"/>
+      <c r="K14" s="170"/>
+      <c r="L14" s="170"/>
+      <c r="M14" s="170"/>
+      <c r="N14" s="170"/>
+      <c r="O14" s="170"/>
+      <c r="P14" s="170"/>
+      <c r="Q14" s="170"/>
+      <c r="R14" s="170"/>
+      <c r="S14" s="170"/>
+      <c r="T14" s="170"/>
+      <c r="U14" s="170"/>
+      <c r="V14" s="170"/>
+    </row>
+    <row r="15" spans="1:22" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
         <v>188</v>
       </c>
@@ -16099,22 +16128,25 @@
         <v>0</v>
       </c>
       <c r="H15" s="63" t="s">
+        <v>1627</v>
+      </c>
+      <c r="I15" s="63" t="s">
         <v>575</v>
       </c>
-      <c r="I15" s="108" t="s">
+      <c r="J15" s="108" t="s">
         <v>576</v>
       </c>
-      <c r="J15" s="108" t="s">
+      <c r="K15" s="108" t="s">
         <v>577</v>
       </c>
-      <c r="K15" s="106" t="s">
+      <c r="L15" s="106" t="s">
         <v>578</v>
       </c>
-      <c r="L15" s="86"/>
-      <c r="M15" s="63" t="s">
-        <v>51</v>
-      </c>
+      <c r="M15" s="86"/>
       <c r="N15" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="O15" s="63" t="s">
         <v>535</v>
       </c>
     </row>
@@ -16136,20 +16168,23 @@
       <c r="G16" s="106" t="b">
         <v>0</v>
       </c>
-      <c r="H16" s="157" t="s">
+      <c r="H16" s="63" t="s">
+        <v>1627</v>
+      </c>
+      <c r="I16" s="157" t="s">
         <v>581</v>
       </c>
-      <c r="I16" s="108" t="s">
+      <c r="J16" s="108" t="s">
         <v>576</v>
       </c>
-      <c r="J16" s="108"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="86"/>
-      <c r="N16" s="63" t="s">
+      <c r="K16" s="108"/>
+      <c r="L16" s="106"/>
+      <c r="M16" s="86"/>
+      <c r="O16" s="63" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="63" t="s">
         <v>188</v>
       </c>
@@ -16165,20 +16200,23 @@
       <c r="G17" s="106" t="b">
         <v>0</v>
       </c>
-      <c r="H17" s="157" t="s">
+      <c r="H17" s="63" t="s">
+        <v>1627</v>
+      </c>
+      <c r="I17" s="157" t="s">
         <v>583</v>
       </c>
-      <c r="I17" s="108" t="s">
+      <c r="J17" s="108" t="s">
         <v>576</v>
       </c>
-      <c r="J17" s="108"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="86"/>
-      <c r="N17" s="63" t="s">
+      <c r="K17" s="108"/>
+      <c r="L17" s="106"/>
+      <c r="M17" s="86"/>
+      <c r="O17" s="63" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="63" t="s">
         <v>188</v>
       </c>
@@ -16198,26 +16236,29 @@
         <v>0</v>
       </c>
       <c r="H18" s="63" t="s">
+        <v>1627</v>
+      </c>
+      <c r="I18" s="63" t="s">
         <v>586</v>
       </c>
-      <c r="I18" s="108" t="s">
+      <c r="J18" s="108" t="s">
         <v>576</v>
       </c>
-      <c r="J18" s="108" t="s">
+      <c r="K18" s="108" t="s">
         <v>577</v>
       </c>
-      <c r="K18" s="106" t="s">
+      <c r="L18" s="106" t="s">
         <v>578</v>
       </c>
-      <c r="L18" s="86"/>
-      <c r="M18" s="63" t="s">
-        <v>51</v>
-      </c>
+      <c r="M18" s="86"/>
       <c r="N18" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="O18" s="63" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="63" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" s="63" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="63" t="s">
         <v>188</v>
       </c>
@@ -16240,26 +16281,29 @@
         <v>0</v>
       </c>
       <c r="H19" s="63" t="s">
+        <v>1627</v>
+      </c>
+      <c r="I19" s="63" t="s">
         <v>588</v>
       </c>
-      <c r="I19" s="108" t="s">
+      <c r="J19" s="108" t="s">
         <v>576</v>
       </c>
-      <c r="J19" s="108" t="s">
+      <c r="K19" s="108" t="s">
         <v>577</v>
       </c>
-      <c r="K19" s="106" t="s">
+      <c r="L19" s="106" t="s">
         <v>578</v>
       </c>
-      <c r="L19" s="86"/>
-      <c r="M19" s="63" t="s">
-        <v>51</v>
-      </c>
+      <c r="M19" s="86"/>
       <c r="N19" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="O19" s="63" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="63" t="s">
         <v>188</v>
       </c>
@@ -16278,27 +16322,30 @@
       <c r="G20" s="106" t="b">
         <v>0</v>
       </c>
-      <c r="H20" s="157" t="s">
+      <c r="H20" s="63" t="s">
+        <v>1627</v>
+      </c>
+      <c r="I20" s="157" t="s">
         <v>590</v>
       </c>
-      <c r="I20" s="108" t="s">
+      <c r="J20" s="108" t="s">
         <v>576</v>
       </c>
-      <c r="J20" s="108" t="s">
+      <c r="K20" s="108" t="s">
         <v>577</v>
       </c>
-      <c r="K20" s="106" t="s">
+      <c r="L20" s="106" t="s">
         <v>578</v>
       </c>
-      <c r="L20" s="86"/>
-      <c r="M20" s="63" t="s">
-        <v>51</v>
-      </c>
+      <c r="M20" s="86"/>
       <c r="N20" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="O20" s="63" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
         <v>189</v>
       </c>
@@ -16315,19 +16362,22 @@
         <v>1</v>
       </c>
       <c r="H21" s="63" t="s">
+        <v>1628</v>
+      </c>
+      <c r="I21" s="63" t="s">
         <v>591</v>
       </c>
-      <c r="I21" s="108" t="s">
+      <c r="J21" s="108" t="s">
         <v>576</v>
       </c>
-      <c r="J21" s="108"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="86"/>
-      <c r="N21" s="63" t="s">
+      <c r="K21" s="108"/>
+      <c r="L21" s="106"/>
+      <c r="M21" s="86"/>
+      <c r="O21" s="63" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="63" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="63" t="s">
         <v>189</v>
       </c>
@@ -16344,19 +16394,22 @@
         <v>0</v>
       </c>
       <c r="H22" s="63" t="s">
+        <v>1628</v>
+      </c>
+      <c r="I22" s="63" t="s">
         <v>592</v>
       </c>
-      <c r="I22" s="108">
+      <c r="J22" s="108">
         <v>8</v>
       </c>
-      <c r="J22" s="108"/>
-      <c r="K22" s="106"/>
-      <c r="L22" s="86"/>
-      <c r="N22" s="63" t="s">
+      <c r="K22" s="108"/>
+      <c r="L22" s="106"/>
+      <c r="M22" s="86"/>
+      <c r="O22" s="63" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="63" t="s">
         <v>190</v>
       </c>
@@ -16373,19 +16426,22 @@
         <v>0</v>
       </c>
       <c r="H23" s="63" t="s">
+        <v>1628</v>
+      </c>
+      <c r="I23" s="63" t="s">
         <v>591</v>
       </c>
-      <c r="I23" s="108" t="s">
+      <c r="J23" s="108" t="s">
         <v>576</v>
       </c>
-      <c r="J23" s="108"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="86"/>
-      <c r="N23" s="63" t="s">
+      <c r="K23" s="108"/>
+      <c r="L23" s="106"/>
+      <c r="M23" s="86"/>
+      <c r="O23" s="63" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="63" t="s">
         <v>190</v>
       </c>
@@ -16402,15 +16458,18 @@
         <v>0</v>
       </c>
       <c r="H24" s="63" t="s">
+        <v>1628</v>
+      </c>
+      <c r="I24" s="63" t="s">
         <v>592</v>
       </c>
-      <c r="I24" s="108">
+      <c r="J24" s="108">
         <v>8</v>
       </c>
-      <c r="J24" s="108"/>
-      <c r="K24" s="106"/>
-      <c r="L24" s="86"/>
-      <c r="N24" s="63" t="s">
+      <c r="K24" s="108"/>
+      <c r="L24" s="106"/>
+      <c r="M24" s="86"/>
+      <c r="O24" s="63" t="s">
         <v>535</v>
       </c>
     </row>
@@ -16973,9 +17032,9 @@
     <mergeCell ref="D14:V14"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H16" r:id="rId1" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
-    <hyperlink ref="H17" r:id="rId2" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
-    <hyperlink ref="H20" r:id="rId3" xr:uid="{00000000-0004-0000-1400-000002000000}"/>
+    <hyperlink ref="I16" r:id="rId1" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="I17" r:id="rId2" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
+    <hyperlink ref="I20" r:id="rId3" xr:uid="{00000000-0004-0000-1400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -17909,7 +17968,7 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="146" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="B15" s="146" t="s">
         <v>685</v>
@@ -22488,7 +22547,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="146" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="B39" s="146" t="s">
         <v>51</v>
@@ -22685,7 +22744,7 @@
     </row>
     <row r="15" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>864</v>
@@ -22762,7 +22821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
@@ -22772,9 +22831,9 @@
     <col min="1" max="1" width="26.85546875" style="10" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" style="68" customWidth="1"/>
     <col min="3" max="3" width="39" style="10" customWidth="1"/>
-    <col min="4" max="4" width="39" style="166" customWidth="1"/>
+    <col min="4" max="4" width="39" style="165" customWidth="1"/>
     <col min="5" max="5" width="37" style="10" customWidth="1"/>
-    <col min="6" max="6" width="55.42578125" style="166" customWidth="1"/>
+    <col min="6" max="6" width="55.42578125" style="165" customWidth="1"/>
     <col min="7" max="7" width="38.42578125" style="10" customWidth="1"/>
     <col min="8" max="8" width="27.85546875" style="152" customWidth="1"/>
     <col min="9" max="9" width="38.42578125" style="10" customWidth="1"/>
@@ -22793,14 +22852,14 @@
       <c r="C1" s="9" t="s">
         <v>872</v>
       </c>
-      <c r="D1" s="161" t="s">
-        <v>1623</v>
+      <c r="D1" s="160" t="s">
+        <v>1622</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>873</v>
       </c>
-      <c r="F1" s="161" t="s">
-        <v>1625</v>
+      <c r="F1" s="160" t="s">
+        <v>1624</v>
       </c>
       <c r="G1" s="153" t="s">
         <v>874</v>
@@ -22826,8 +22885,8 @@
         <v>879</v>
       </c>
       <c r="B2" s="114"/>
-      <c r="D2" s="162"/>
-      <c r="F2" s="162"/>
+      <c r="D2" s="161"/>
+      <c r="F2" s="161"/>
       <c r="G2" s="129"/>
       <c r="H2" s="129"/>
       <c r="I2" s="129"/>
@@ -22839,8 +22898,8 @@
         <v>880</v>
       </c>
       <c r="B3" s="115"/>
-      <c r="D3" s="163"/>
-      <c r="F3" s="163"/>
+      <c r="D3" s="162"/>
+      <c r="F3" s="162"/>
       <c r="G3" s="130"/>
       <c r="H3" s="130"/>
       <c r="I3" s="130"/>
@@ -22853,8 +22912,8 @@
         <v>20</v>
       </c>
       <c r="B4" s="115"/>
-      <c r="D4" s="163"/>
-      <c r="F4" s="163"/>
+      <c r="D4" s="162"/>
+      <c r="F4" s="162"/>
       <c r="G4" s="130"/>
       <c r="H4" s="130"/>
       <c r="I4" s="130"/>
@@ -22867,8 +22926,8 @@
         <v>199</v>
       </c>
       <c r="B5" s="115"/>
-      <c r="D5" s="163"/>
-      <c r="F5" s="163"/>
+      <c r="D5" s="162"/>
+      <c r="F5" s="162"/>
       <c r="G5" s="130"/>
       <c r="H5" s="130"/>
       <c r="I5" s="130"/>
@@ -22883,9 +22942,9 @@
       <c r="A6" s="26"/>
       <c r="B6" s="115"/>
       <c r="C6" s="23"/>
-      <c r="D6" s="164"/>
+      <c r="D6" s="163"/>
       <c r="E6" s="23"/>
-      <c r="F6" s="164"/>
+      <c r="F6" s="163"/>
       <c r="G6" s="132"/>
       <c r="H6" s="133"/>
       <c r="I6" s="132"/>
@@ -22905,14 +22964,14 @@
       <c r="C7" s="46" t="s">
         <v>883</v>
       </c>
-      <c r="D7" s="165" t="s">
-        <v>1624</v>
+      <c r="D7" s="164" t="s">
+        <v>1623</v>
       </c>
       <c r="E7" s="46" t="s">
         <v>884</v>
       </c>
-      <c r="F7" s="165" t="s">
-        <v>1626</v>
+      <c r="F7" s="164" t="s">
+        <v>1625</v>
       </c>
       <c r="G7" s="136" t="s">
         <v>885</v>
@@ -22939,9 +22998,9 @@
       <c r="A8" s="26"/>
       <c r="B8" s="115"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="164"/>
+      <c r="D8" s="163"/>
       <c r="E8" s="23"/>
-      <c r="F8" s="164"/>
+      <c r="F8" s="163"/>
       <c r="G8" s="133"/>
       <c r="H8" s="133"/>
       <c r="I8" s="133"/>
@@ -22955,9 +23014,9 @@
     <row r="10" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="68"/>
       <c r="C10" s="21"/>
-      <c r="D10" s="167"/>
+      <c r="D10" s="166"/>
       <c r="E10" s="21"/>
-      <c r="F10" s="167"/>
+      <c r="F10" s="166"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
@@ -22967,7 +23026,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="21"/>
-      <c r="D11" s="167"/>
+      <c r="D11" s="166"/>
       <c r="H11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
@@ -22976,9 +23035,9 @@
       <c r="A12" s="21"/>
       <c r="B12" s="116"/>
       <c r="C12" s="21"/>
-      <c r="D12" s="167"/>
+      <c r="D12" s="166"/>
       <c r="E12" s="15"/>
-      <c r="F12" s="169"/>
+      <c r="F12" s="168"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
@@ -22988,21 +23047,21 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="21"/>
-      <c r="D13" s="167"/>
+      <c r="D13" s="166"/>
     </row>
     <row r="14" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="116"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="167"/>
+      <c r="D14" s="166"/>
       <c r="E14" s="15"/>
-      <c r="F14" s="169"/>
+      <c r="F14" s="168"/>
       <c r="H14" s="152"/>
       <c r="J14" s="152"/>
       <c r="K14" s="152"/>
       <c r="L14" s="10"/>
     </row>
-    <row r="15" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>889</v>
       </c>
@@ -23012,12 +23071,12 @@
       <c r="C15" s="21" t="s">
         <v>891</v>
       </c>
-      <c r="D15" s="167"/>
+      <c r="D15" s="166"/>
       <c r="E15" s="15" t="s">
         <v>868</v>
       </c>
-      <c r="F15" s="170" t="s">
-        <v>1627</v>
+      <c r="F15" s="169" t="s">
+        <v>1626</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>51</v>
@@ -23033,9 +23092,9 @@
       <c r="A16" s="21"/>
       <c r="B16" s="116"/>
       <c r="C16" s="21"/>
-      <c r="D16" s="167"/>
+      <c r="D16" s="166"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="169"/>
+      <c r="F16" s="168"/>
       <c r="H16" s="152"/>
       <c r="J16" s="152"/>
       <c r="K16" s="152"/>
@@ -23043,33 +23102,33 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C17" s="21"/>
-      <c r="D17" s="167"/>
+      <c r="D17" s="166"/>
     </row>
     <row r="18" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="68"/>
-      <c r="D18" s="168"/>
-      <c r="F18" s="168"/>
+      <c r="D18" s="167"/>
+      <c r="F18" s="167"/>
       <c r="L18" s="10"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C19" s="21"/>
-      <c r="D19" s="167"/>
+      <c r="D19" s="166"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="116"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="167"/>
+      <c r="D20" s="166"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C21" s="21"/>
-      <c r="D21" s="167"/>
+      <c r="D21" s="166"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="116"/>
       <c r="C22" s="21"/>
-      <c r="D22" s="167"/>
+      <c r="D22" s="166"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24305,7 +24364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AL49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
@@ -25939,7 +25998,7 @@
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>51</v>
@@ -26022,7 +26081,7 @@
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>51</v>
@@ -26117,7 +26176,7 @@
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>51</v>
@@ -29466,7 +29525,7 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>1190</v>
@@ -29510,7 +29569,7 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>1192</v>
@@ -29554,7 +29613,7 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>1193</v>
@@ -29598,7 +29657,7 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>1190</v>
@@ -29642,7 +29701,7 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>1192</v>
@@ -29686,7 +29745,7 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>1193</v>
@@ -32497,7 +32556,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>1234</v>
@@ -32532,7 +32591,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>1234</v>
@@ -32567,7 +32626,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>1234</v>
@@ -34804,7 +34863,7 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>1332</v>
@@ -34819,10 +34878,10 @@
         <v>103</v>
       </c>
       <c r="F15" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="G15" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="H15" t="s">
         <v>103</v>
@@ -34845,7 +34904,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B16" s="59" t="s">
         <v>1332</v>
@@ -34877,7 +34936,7 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B17" s="59" t="s">
         <v>1332</v>
@@ -34892,10 +34951,10 @@
         <v>103</v>
       </c>
       <c r="F17" t="s">
+        <v>1619</v>
+      </c>
+      <c r="G17" t="s">
         <v>1620</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1621</v>
       </c>
       <c r="H17" t="s">
         <v>103</v>
@@ -34918,7 +34977,7 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B18" s="59" t="s">
         <v>1332</v>
@@ -34933,10 +34992,10 @@
         <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="G18" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="H18" t="s">
         <v>103</v>
@@ -34959,7 +35018,7 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B19" s="59" t="s">
         <v>1332</v>
@@ -35021,7 +35080,7 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B20" s="59" t="s">
         <v>1332</v>
@@ -35062,7 +35121,7 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B21" s="59" t="s">
         <v>1332</v>
@@ -35103,7 +35162,7 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B22" s="59" t="s">
         <v>1332</v>
@@ -35144,7 +35203,7 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B23" s="59" t="s">
         <v>1332</v>
@@ -35179,7 +35238,7 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B24" s="59" t="s">
         <v>1332</v>
@@ -35272,9 +35331,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -35630,12 +35689,6 @@
     <row r="15" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>790</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>1094</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>1092</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>947</v>
@@ -38105,9 +38158,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5476BCB0-492A-4349-9B4C-02D8DB45D26B}">
   <dimension ref="A1:T116"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38121,8 +38174,9 @@
     <col min="8" max="8" width="40.7109375" style="10" customWidth="1"/>
     <col min="9" max="9" width="33.140625" style="10" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" style="10" customWidth="1"/>
-    <col min="11" max="11" width="33.140625" style="10" customWidth="1"/>
-    <col min="12" max="13" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="24.5703125" style="165" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" style="165" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" customWidth="1"/>
     <col min="14" max="14" width="23" customWidth="1"/>
     <col min="15" max="15" width="18.42578125" customWidth="1"/>
     <col min="16" max="16" width="18.42578125" style="10" customWidth="1"/>
@@ -38162,11 +38216,11 @@
       <c r="J1" s="11" t="s">
         <v>1134</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>1135</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>1017</v>
+      <c r="K1" s="171" t="s">
+        <v>1629</v>
+      </c>
+      <c r="L1" s="171" t="s">
+        <v>1630</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>1136</v>
@@ -38202,7 +38256,8 @@
       <c r="G2" s="38"/>
       <c r="I2" s="38"/>
       <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
+      <c r="K2" s="172"/>
+      <c r="L2" s="172"/>
     </row>
     <row r="3" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
@@ -38212,7 +38267,8 @@
       <c r="G3" s="27"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
+      <c r="K3" s="173"/>
+      <c r="L3" s="173"/>
     </row>
     <row r="4" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
@@ -38222,7 +38278,8 @@
       <c r="G4" s="27"/>
       <c r="I4" s="27"/>
       <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
+      <c r="K4" s="173"/>
+      <c r="L4" s="173"/>
     </row>
     <row r="5" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="61" t="s">
@@ -38232,7 +38289,8 @@
       <c r="G5" s="27"/>
       <c r="I5" s="27"/>
       <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
+      <c r="K5" s="173"/>
+      <c r="L5" s="173"/>
     </row>
     <row r="6" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
@@ -38242,8 +38300,8 @@
       <c r="G6" s="27"/>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
+      <c r="K6" s="173"/>
+      <c r="L6" s="173"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
       <c r="S6" s="27"/>
@@ -38258,8 +38316,8 @@
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
+      <c r="K7" s="163"/>
+      <c r="L7" s="163"/>
       <c r="M7" s="23"/>
       <c r="N7" s="23"/>
       <c r="Q7" s="23"/>
@@ -38297,11 +38355,11 @@
       <c r="J8" s="54" t="s">
         <v>1155</v>
       </c>
-      <c r="K8" s="54" t="s">
-        <v>1429</v>
-      </c>
-      <c r="L8" s="54" t="s">
-        <v>1157</v>
+      <c r="K8" s="174" t="s">
+        <v>1631</v>
+      </c>
+      <c r="L8" s="174" t="s">
+        <v>1632</v>
       </c>
       <c r="M8" s="45" t="s">
         <v>1158</v>
@@ -38324,6 +38382,22 @@
       <c r="S8" s="53" t="s">
         <v>817</v>
       </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K11" s="175"/>
+      <c r="L11" s="175"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K12" s="175"/>
+      <c r="L12" s="175"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K13" s="175"/>
+      <c r="L13" s="175"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="K14" s="175"/>
+      <c r="L14" s="175"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
@@ -38356,14 +38430,10 @@
       <c r="J15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L15" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K15" s="175"/>
+      <c r="L15" s="175"/>
       <c r="M15" s="159" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="N15" t="s">
         <v>1060</v>
@@ -38415,14 +38485,10 @@
       <c r="J16" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L16" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K16" s="175"/>
+      <c r="L16" s="175"/>
       <c r="M16" s="159" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="N16" t="s">
         <v>1060</v>
@@ -38474,23 +38540,19 @@
       <c r="J17" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K17" s="175"/>
+      <c r="L17" s="175"/>
       <c r="M17" s="159" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="N17" t="s">
         <v>1060</v>
       </c>
       <c r="O17" t="s">
+        <v>1432</v>
+      </c>
+      <c r="P17" s="10" t="s">
         <v>1433</v>
-      </c>
-      <c r="P17" s="10" t="s">
-        <v>1434</v>
       </c>
       <c r="Q17" s="10" t="s">
         <v>51</v>
@@ -38533,23 +38595,19 @@
       <c r="J18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L18" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K18" s="175"/>
+      <c r="L18" s="175"/>
       <c r="M18" s="159" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="N18" t="s">
         <v>1060</v>
       </c>
       <c r="O18" t="s">
+        <v>1435</v>
+      </c>
+      <c r="P18" s="10" t="s">
         <v>1436</v>
-      </c>
-      <c r="P18" s="10" t="s">
-        <v>1437</v>
       </c>
       <c r="Q18" s="10" t="s">
         <v>51</v>
@@ -38592,14 +38650,10 @@
       <c r="J19" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K19" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L19" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K19" s="175"/>
+      <c r="L19" s="175"/>
       <c r="M19" s="159" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="N19" t="s">
         <v>1060</v>
@@ -38651,14 +38705,10 @@
       <c r="J20" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K20" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K20" s="175"/>
+      <c r="L20" s="175"/>
       <c r="M20" s="159" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="N20" t="s">
         <v>1060</v>
@@ -38710,14 +38760,10 @@
       <c r="J21" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L21" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K21" s="175"/>
+      <c r="L21" s="175"/>
       <c r="M21" s="159" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="N21" t="s">
         <v>1060</v>
@@ -38769,14 +38815,10 @@
       <c r="J22" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K22" s="175"/>
+      <c r="L22" s="175"/>
       <c r="M22" s="159" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="N22" t="s">
         <v>1060</v>
@@ -38828,14 +38870,10 @@
       <c r="J23" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K23" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K23" s="175"/>
+      <c r="L23" s="175"/>
       <c r="M23" s="159" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="N23" t="s">
         <v>1060</v>
@@ -38887,14 +38925,10 @@
       <c r="J24" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K24" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L24" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K24" s="175"/>
+      <c r="L24" s="175"/>
       <c r="M24" s="159" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="N24" t="s">
         <v>1060</v>
@@ -38946,23 +38980,19 @@
       <c r="J25" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K25" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L25" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K25" s="175"/>
+      <c r="L25" s="175"/>
       <c r="M25" s="159" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="N25" t="s">
         <v>1060</v>
       </c>
       <c r="O25" t="s">
+        <v>1444</v>
+      </c>
+      <c r="P25" s="10" t="s">
         <v>1445</v>
-      </c>
-      <c r="P25" s="10" t="s">
-        <v>1446</v>
       </c>
       <c r="Q25" s="10" t="s">
         <v>51</v>
@@ -39005,23 +39035,19 @@
       <c r="J26" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K26" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L26" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K26" s="175"/>
+      <c r="L26" s="175"/>
       <c r="M26" s="159" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="N26" t="s">
         <v>1060</v>
       </c>
       <c r="O26" t="s">
+        <v>1447</v>
+      </c>
+      <c r="P26" s="10" t="s">
         <v>1448</v>
-      </c>
-      <c r="P26" s="10" t="s">
-        <v>1449</v>
       </c>
       <c r="Q26" s="10" t="s">
         <v>51</v>
@@ -39064,14 +39090,10 @@
       <c r="J27" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K27" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L27" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K27" s="175"/>
+      <c r="L27" s="175"/>
       <c r="M27" s="159" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="N27" t="s">
         <v>1060</v>
@@ -39123,14 +39145,10 @@
       <c r="J28" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K28" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L28" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K28" s="175"/>
+      <c r="L28" s="175"/>
       <c r="M28" s="159" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="N28" t="s">
         <v>1060</v>
@@ -39182,23 +39200,19 @@
       <c r="J29" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K29" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L29" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K29" s="175"/>
+      <c r="L29" s="175"/>
       <c r="M29" s="159" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="N29" t="s">
         <v>1060</v>
       </c>
       <c r="O29" t="s">
+        <v>1452</v>
+      </c>
+      <c r="P29" s="10" t="s">
         <v>1453</v>
-      </c>
-      <c r="P29" s="10" t="s">
-        <v>1454</v>
       </c>
       <c r="Q29" s="10" t="s">
         <v>51</v>
@@ -39241,23 +39255,19 @@
       <c r="J30" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K30" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L30" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K30" s="175"/>
+      <c r="L30" s="175"/>
       <c r="M30" s="159" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="N30" t="s">
         <v>1060</v>
       </c>
       <c r="O30" t="s">
+        <v>1455</v>
+      </c>
+      <c r="P30" s="10" t="s">
         <v>1456</v>
-      </c>
-      <c r="P30" s="10" t="s">
-        <v>1457</v>
       </c>
       <c r="Q30" s="10" t="s">
         <v>51</v>
@@ -39300,14 +39310,10 @@
       <c r="J31" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K31" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L31" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K31" s="175"/>
+      <c r="L31" s="175"/>
       <c r="M31" s="159" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="N31" t="s">
         <v>1060</v>
@@ -39359,14 +39365,10 @@
       <c r="J32" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K32" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L32" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K32" s="175"/>
+      <c r="L32" s="175"/>
       <c r="M32" s="159" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="N32" t="s">
         <v>1060</v>
@@ -39418,23 +39420,19 @@
       <c r="J33" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K33" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L33" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K33" s="175"/>
+      <c r="L33" s="175"/>
       <c r="M33" s="159" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="N33" t="s">
         <v>1060</v>
       </c>
       <c r="O33" t="s">
+        <v>1460</v>
+      </c>
+      <c r="P33" s="10" t="s">
         <v>1461</v>
-      </c>
-      <c r="P33" s="10" t="s">
-        <v>1462</v>
       </c>
       <c r="Q33" s="10" t="s">
         <v>51</v>
@@ -39477,23 +39475,19 @@
       <c r="J34" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K34" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L34" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K34" s="175"/>
+      <c r="L34" s="175"/>
       <c r="M34" s="159" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="N34" t="s">
         <v>1060</v>
       </c>
       <c r="O34" t="s">
+        <v>1463</v>
+      </c>
+      <c r="P34" s="10" t="s">
         <v>1464</v>
-      </c>
-      <c r="P34" s="10" t="s">
-        <v>1465</v>
       </c>
       <c r="Q34" s="10" t="s">
         <v>51</v>
@@ -39536,14 +39530,10 @@
       <c r="J35" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L35" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K35" s="175"/>
+      <c r="L35" s="175"/>
       <c r="M35" s="159" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="N35" t="s">
         <v>1060</v>
@@ -39595,14 +39585,10 @@
       <c r="J36" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K36" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L36" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K36" s="175"/>
+      <c r="L36" s="175"/>
       <c r="M36" s="159" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="N36" t="s">
         <v>1060</v>
@@ -39654,23 +39640,19 @@
       <c r="J37" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K37" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L37" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K37" s="175"/>
+      <c r="L37" s="175"/>
       <c r="M37" s="159" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="N37" t="s">
         <v>1060</v>
       </c>
       <c r="O37" t="s">
+        <v>1468</v>
+      </c>
+      <c r="P37" s="10" t="s">
         <v>1469</v>
-      </c>
-      <c r="P37" s="10" t="s">
-        <v>1470</v>
       </c>
       <c r="Q37" s="10" t="s">
         <v>51</v>
@@ -39713,23 +39695,19 @@
       <c r="J38" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K38" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L38" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K38" s="175"/>
+      <c r="L38" s="175"/>
       <c r="M38" s="159" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="N38" t="s">
         <v>1060</v>
       </c>
       <c r="O38" t="s">
+        <v>1471</v>
+      </c>
+      <c r="P38" s="10" t="s">
         <v>1472</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>1473</v>
       </c>
       <c r="Q38" s="10" t="s">
         <v>51</v>
@@ -39772,14 +39750,10 @@
       <c r="J39" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K39" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L39" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K39" s="175"/>
+      <c r="L39" s="175"/>
       <c r="M39" s="159" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="N39" t="s">
         <v>1060</v>
@@ -39831,14 +39805,10 @@
       <c r="J40" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K40" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L40" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K40" s="175"/>
+      <c r="L40" s="175"/>
       <c r="M40" s="159" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="N40" t="s">
         <v>1060</v>
@@ -39890,23 +39860,19 @@
       <c r="J41" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K41" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L41" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K41" s="175"/>
+      <c r="L41" s="175"/>
       <c r="M41" s="159" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="N41" t="s">
         <v>1060</v>
       </c>
       <c r="O41" t="s">
+        <v>1476</v>
+      </c>
+      <c r="P41" s="10" t="s">
         <v>1477</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>1478</v>
       </c>
       <c r="Q41" s="10" t="s">
         <v>51</v>
@@ -39949,23 +39915,19 @@
       <c r="J42" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K42" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L42" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K42" s="175"/>
+      <c r="L42" s="175"/>
       <c r="M42" s="159" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="N42" t="s">
         <v>1060</v>
       </c>
       <c r="O42" t="s">
+        <v>1479</v>
+      </c>
+      <c r="P42" s="10" t="s">
         <v>1480</v>
-      </c>
-      <c r="P42" s="10" t="s">
-        <v>1481</v>
       </c>
       <c r="Q42" s="10" t="s">
         <v>51</v>
@@ -40008,14 +39970,10 @@
       <c r="J43" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K43" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L43" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K43" s="175"/>
+      <c r="L43" s="175"/>
       <c r="M43" s="159" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="N43" t="s">
         <v>1060</v>
@@ -40067,14 +40025,10 @@
       <c r="J44" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K44" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L44" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K44" s="175"/>
+      <c r="L44" s="175"/>
       <c r="M44" s="159" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="N44" t="s">
         <v>1060</v>
@@ -40126,23 +40080,19 @@
       <c r="J45" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K45" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L45" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K45" s="175"/>
+      <c r="L45" s="175"/>
       <c r="M45" s="159" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="N45" t="s">
         <v>1060</v>
       </c>
       <c r="O45" t="s">
+        <v>1484</v>
+      </c>
+      <c r="P45" s="10" t="s">
         <v>1485</v>
-      </c>
-      <c r="P45" s="10" t="s">
-        <v>1486</v>
       </c>
       <c r="Q45" s="10" t="s">
         <v>51</v>
@@ -40185,23 +40135,19 @@
       <c r="J46" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K46" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L46" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K46" s="175"/>
+      <c r="L46" s="175"/>
       <c r="M46" s="159" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="N46" t="s">
         <v>1060</v>
       </c>
       <c r="O46" t="s">
+        <v>1487</v>
+      </c>
+      <c r="P46" s="10" t="s">
         <v>1488</v>
-      </c>
-      <c r="P46" s="10" t="s">
-        <v>1489</v>
       </c>
       <c r="Q46" s="10" t="s">
         <v>51</v>
@@ -40244,14 +40190,10 @@
       <c r="J47" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K47" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L47" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K47" s="175"/>
+      <c r="L47" s="175"/>
       <c r="M47" s="159" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="N47" t="s">
         <v>1060</v>
@@ -40303,14 +40245,10 @@
       <c r="J48" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K48" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L48" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K48" s="175"/>
+      <c r="L48" s="175"/>
       <c r="M48" s="159" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="N48" t="s">
         <v>1060</v>
@@ -40362,23 +40300,19 @@
       <c r="J49" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K49" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L49" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K49" s="175"/>
+      <c r="L49" s="175"/>
       <c r="M49" s="159" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="N49" t="s">
         <v>1060</v>
       </c>
       <c r="O49" t="s">
+        <v>1492</v>
+      </c>
+      <c r="P49" s="10" t="s">
         <v>1493</v>
-      </c>
-      <c r="P49" s="10" t="s">
-        <v>1494</v>
       </c>
       <c r="Q49" s="10" t="s">
         <v>51</v>
@@ -40421,23 +40355,19 @@
       <c r="J50" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K50" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L50" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K50" s="175"/>
+      <c r="L50" s="175"/>
       <c r="M50" s="159" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="N50" t="s">
         <v>1060</v>
       </c>
       <c r="O50" t="s">
+        <v>1495</v>
+      </c>
+      <c r="P50" s="10" t="s">
         <v>1496</v>
-      </c>
-      <c r="P50" s="10" t="s">
-        <v>1497</v>
       </c>
       <c r="Q50" s="10" t="s">
         <v>51</v>
@@ -40480,14 +40410,10 @@
       <c r="J51" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K51" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L51" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K51" s="175"/>
+      <c r="L51" s="175"/>
       <c r="M51" s="159" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="N51" t="s">
         <v>1060</v>
@@ -40539,14 +40465,10 @@
       <c r="J52" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L52" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K52" s="175"/>
+      <c r="L52" s="175"/>
       <c r="M52" s="159" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="N52" t="s">
         <v>1060</v>
@@ -40598,23 +40520,19 @@
       <c r="J53" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K53" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L53" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K53" s="175"/>
+      <c r="L53" s="175"/>
       <c r="M53" s="159" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="N53" t="s">
         <v>1060</v>
       </c>
       <c r="O53" t="s">
+        <v>1500</v>
+      </c>
+      <c r="P53" s="10" t="s">
         <v>1501</v>
-      </c>
-      <c r="P53" s="10" t="s">
-        <v>1502</v>
       </c>
       <c r="Q53" s="10" t="s">
         <v>51</v>
@@ -40657,23 +40575,19 @@
       <c r="J54" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K54" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L54" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K54" s="175"/>
+      <c r="L54" s="175"/>
       <c r="M54" s="159" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="N54" t="s">
         <v>1060</v>
       </c>
       <c r="O54" t="s">
+        <v>1503</v>
+      </c>
+      <c r="P54" s="10" t="s">
         <v>1504</v>
-      </c>
-      <c r="P54" s="10" t="s">
-        <v>1505</v>
       </c>
       <c r="Q54" s="10" t="s">
         <v>51</v>
@@ -40716,14 +40630,10 @@
       <c r="J55" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K55" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L55" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K55" s="175"/>
+      <c r="L55" s="175"/>
       <c r="M55" s="159" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="N55" t="s">
         <v>1060</v>
@@ -40775,14 +40685,10 @@
       <c r="J56" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K56" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L56" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K56" s="175"/>
+      <c r="L56" s="175"/>
       <c r="M56" s="159" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="N56" t="s">
         <v>1060</v>
@@ -40834,23 +40740,19 @@
       <c r="J57" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K57" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L57" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K57" s="175"/>
+      <c r="L57" s="175"/>
       <c r="M57" s="159" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="N57" t="s">
         <v>1060</v>
       </c>
       <c r="O57" t="s">
+        <v>1508</v>
+      </c>
+      <c r="P57" s="10" t="s">
         <v>1509</v>
-      </c>
-      <c r="P57" s="10" t="s">
-        <v>1510</v>
       </c>
       <c r="Q57" s="10" t="s">
         <v>51</v>
@@ -40893,23 +40795,19 @@
       <c r="J58" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K58" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L58" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K58" s="175"/>
+      <c r="L58" s="175"/>
       <c r="M58" s="159" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="N58" t="s">
         <v>1060</v>
       </c>
       <c r="O58" t="s">
+        <v>1511</v>
+      </c>
+      <c r="P58" s="10" t="s">
         <v>1512</v>
-      </c>
-      <c r="P58" s="10" t="s">
-        <v>1513</v>
       </c>
       <c r="Q58" s="10" t="s">
         <v>51</v>
@@ -40952,14 +40850,10 @@
       <c r="J59" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K59" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L59" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K59" s="175"/>
+      <c r="L59" s="175"/>
       <c r="M59" s="159" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="N59" t="s">
         <v>1060</v>
@@ -41011,14 +40905,10 @@
       <c r="J60" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K60" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L60" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K60" s="175"/>
+      <c r="L60" s="175"/>
       <c r="M60" s="159" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="N60" t="s">
         <v>1060</v>
@@ -41070,23 +40960,19 @@
       <c r="J61" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K61" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L61" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K61" s="175"/>
+      <c r="L61" s="175"/>
       <c r="M61" s="159" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="N61" t="s">
         <v>1060</v>
       </c>
       <c r="O61" t="s">
+        <v>1516</v>
+      </c>
+      <c r="P61" s="10" t="s">
         <v>1517</v>
-      </c>
-      <c r="P61" s="10" t="s">
-        <v>1518</v>
       </c>
       <c r="Q61" s="10" t="s">
         <v>51</v>
@@ -41129,23 +41015,19 @@
       <c r="J62" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K62" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L62" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K62" s="175"/>
+      <c r="L62" s="175"/>
       <c r="M62" s="159" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="N62" t="s">
         <v>1060</v>
       </c>
       <c r="O62" t="s">
+        <v>1519</v>
+      </c>
+      <c r="P62" s="10" t="s">
         <v>1520</v>
-      </c>
-      <c r="P62" s="10" t="s">
-        <v>1521</v>
       </c>
       <c r="Q62" s="10" t="s">
         <v>51</v>
@@ -41188,14 +41070,10 @@
       <c r="J63" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K63" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L63" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K63" s="175"/>
+      <c r="L63" s="175"/>
       <c r="M63" s="159" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="N63" t="s">
         <v>1060</v>
@@ -41247,14 +41125,10 @@
       <c r="J64" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K64" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L64" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K64" s="175"/>
+      <c r="L64" s="175"/>
       <c r="M64" s="159" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="N64" t="s">
         <v>1060</v>
@@ -41306,23 +41180,19 @@
       <c r="J65" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K65" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L65" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K65" s="175"/>
+      <c r="L65" s="175"/>
       <c r="M65" s="159" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="N65" t="s">
         <v>1060</v>
       </c>
       <c r="O65" t="s">
+        <v>1524</v>
+      </c>
+      <c r="P65" s="10" t="s">
         <v>1525</v>
-      </c>
-      <c r="P65" s="10" t="s">
-        <v>1526</v>
       </c>
       <c r="Q65" s="10" t="s">
         <v>51</v>
@@ -41365,23 +41235,19 @@
       <c r="J66" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K66" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L66" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K66" s="175"/>
+      <c r="L66" s="175"/>
       <c r="M66" s="159" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="N66" t="s">
         <v>1060</v>
       </c>
       <c r="O66" t="s">
+        <v>1527</v>
+      </c>
+      <c r="P66" s="10" t="s">
         <v>1528</v>
-      </c>
-      <c r="P66" s="10" t="s">
-        <v>1529</v>
       </c>
       <c r="Q66" s="10" t="s">
         <v>51</v>
@@ -41424,14 +41290,10 @@
       <c r="J67" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K67" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L67" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K67" s="175"/>
+      <c r="L67" s="175"/>
       <c r="M67" s="159" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="N67" t="s">
         <v>1060</v>
@@ -41483,14 +41345,10 @@
       <c r="J68" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K68" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L68" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K68" s="175"/>
+      <c r="L68" s="175"/>
       <c r="M68" s="159" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="N68" t="s">
         <v>1060</v>
@@ -41542,23 +41400,19 @@
       <c r="J69" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K69" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L69" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K69" s="175"/>
+      <c r="L69" s="175"/>
       <c r="M69" s="159" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="N69" t="s">
         <v>1060</v>
       </c>
       <c r="O69" t="s">
+        <v>1532</v>
+      </c>
+      <c r="P69" s="10" t="s">
         <v>1533</v>
-      </c>
-      <c r="P69" s="10" t="s">
-        <v>1534</v>
       </c>
       <c r="Q69" s="10" t="s">
         <v>51</v>
@@ -41601,23 +41455,19 @@
       <c r="J70" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K70" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L70" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K70" s="175"/>
+      <c r="L70" s="175"/>
       <c r="M70" s="159" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="N70" t="s">
         <v>1060</v>
       </c>
       <c r="O70" t="s">
+        <v>1535</v>
+      </c>
+      <c r="P70" s="10" t="s">
         <v>1536</v>
-      </c>
-      <c r="P70" s="10" t="s">
-        <v>1537</v>
       </c>
       <c r="Q70" s="10" t="s">
         <v>51</v>
@@ -41660,14 +41510,10 @@
       <c r="J71" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K71" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L71" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K71" s="175"/>
+      <c r="L71" s="175"/>
       <c r="M71" s="159" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="N71" t="s">
         <v>1060</v>
@@ -41719,14 +41565,10 @@
       <c r="J72" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K72" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L72" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K72" s="175"/>
+      <c r="L72" s="175"/>
       <c r="M72" s="159" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="N72" t="s">
         <v>1060</v>
@@ -41778,23 +41620,19 @@
       <c r="J73" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K73" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L73" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K73" s="175"/>
+      <c r="L73" s="175"/>
       <c r="M73" s="159" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="N73" t="s">
         <v>1060</v>
       </c>
       <c r="O73" t="s">
+        <v>1540</v>
+      </c>
+      <c r="P73" s="10" t="s">
         <v>1541</v>
-      </c>
-      <c r="P73" s="10" t="s">
-        <v>1542</v>
       </c>
       <c r="Q73" s="10" t="s">
         <v>51</v>
@@ -41837,23 +41675,19 @@
       <c r="J74" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K74" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L74" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K74" s="175"/>
+      <c r="L74" s="175"/>
       <c r="M74" s="159" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="N74" t="s">
         <v>1060</v>
       </c>
       <c r="O74" t="s">
+        <v>1543</v>
+      </c>
+      <c r="P74" s="10" t="s">
         <v>1544</v>
-      </c>
-      <c r="P74" s="10" t="s">
-        <v>1545</v>
       </c>
       <c r="Q74" s="10" t="s">
         <v>51</v>
@@ -41896,14 +41730,10 @@
       <c r="J75" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K75" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L75" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K75" s="175"/>
+      <c r="L75" s="175"/>
       <c r="M75" s="159" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="N75" t="s">
         <v>1060</v>
@@ -41955,14 +41785,10 @@
       <c r="J76" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K76" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L76" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K76" s="175"/>
+      <c r="L76" s="175"/>
       <c r="M76" s="159" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="N76" t="s">
         <v>1060</v>
@@ -42014,23 +41840,19 @@
       <c r="J77" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K77" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L77" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K77" s="175"/>
+      <c r="L77" s="175"/>
       <c r="M77" s="159" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="N77" t="s">
         <v>1060</v>
       </c>
       <c r="O77" t="s">
+        <v>1548</v>
+      </c>
+      <c r="P77" s="10" t="s">
         <v>1549</v>
-      </c>
-      <c r="P77" s="10" t="s">
-        <v>1550</v>
       </c>
       <c r="Q77" s="10" t="s">
         <v>51</v>
@@ -42073,23 +41895,19 @@
       <c r="J78" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K78" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L78" t="s">
-        <v>1060</v>
-      </c>
+      <c r="K78" s="175"/>
+      <c r="L78" s="175"/>
       <c r="M78" s="159" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="N78" t="s">
         <v>1060</v>
       </c>
       <c r="O78" t="s">
+        <v>1551</v>
+      </c>
+      <c r="P78" s="10" t="s">
         <v>1552</v>
-      </c>
-      <c r="P78" s="10" t="s">
-        <v>1553</v>
       </c>
       <c r="Q78" s="10" t="s">
         <v>51</v>
@@ -42132,14 +41950,8 @@
       <c r="J79" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K79" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L79" t="s">
-        <v>1060</v>
-      </c>
       <c r="M79" s="159" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="N79" t="s">
         <v>1060</v>
@@ -42191,14 +42003,8 @@
       <c r="J80" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K80" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L80" t="s">
-        <v>1060</v>
-      </c>
       <c r="M80" s="159" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="N80" t="s">
         <v>1060</v>
@@ -42250,14 +42056,8 @@
       <c r="J81" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K81" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L81" t="s">
-        <v>1060</v>
-      </c>
       <c r="M81" s="159" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="N81" t="s">
         <v>1060</v>
@@ -42309,14 +42109,8 @@
       <c r="J82" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K82" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L82" t="s">
-        <v>1060</v>
-      </c>
       <c r="M82" s="159" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="N82" t="s">
         <v>1060</v>
@@ -42368,14 +42162,8 @@
       <c r="J83" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K83" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L83" t="s">
-        <v>1060</v>
-      </c>
       <c r="M83" s="159" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="N83" t="s">
         <v>1060</v>
@@ -42427,14 +42215,8 @@
       <c r="J84" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K84" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L84" t="s">
-        <v>1060</v>
-      </c>
       <c r="M84" s="159" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="N84" t="s">
         <v>1060</v>
@@ -42486,23 +42268,17 @@
       <c r="J85" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K85" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L85" t="s">
-        <v>1060</v>
-      </c>
       <c r="M85" s="159" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="N85" t="s">
         <v>1060</v>
       </c>
       <c r="O85" t="s">
+        <v>1560</v>
+      </c>
+      <c r="P85" s="10" t="s">
         <v>1561</v>
-      </c>
-      <c r="P85" s="10" t="s">
-        <v>1562</v>
       </c>
       <c r="Q85" s="10" t="s">
         <v>51</v>
@@ -42545,23 +42321,17 @@
       <c r="J86" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K86" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L86" t="s">
-        <v>1060</v>
-      </c>
       <c r="M86" s="159" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="N86" t="s">
         <v>1060</v>
       </c>
       <c r="O86" t="s">
+        <v>1563</v>
+      </c>
+      <c r="P86" s="10" t="s">
         <v>1564</v>
-      </c>
-      <c r="P86" s="10" t="s">
-        <v>1565</v>
       </c>
       <c r="Q86" s="10" t="s">
         <v>51</v>
@@ -42604,14 +42374,8 @@
       <c r="J87" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K87" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L87" t="s">
-        <v>1060</v>
-      </c>
       <c r="M87" s="159" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="N87" t="s">
         <v>1060</v>
@@ -42663,14 +42427,8 @@
       <c r="J88" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K88" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L88" t="s">
-        <v>1060</v>
-      </c>
       <c r="M88" s="159" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="N88" t="s">
         <v>1060</v>
@@ -42722,14 +42480,8 @@
       <c r="J89" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K89" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L89" t="s">
-        <v>1060</v>
-      </c>
       <c r="M89" s="159" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="N89" t="s">
         <v>1060</v>
@@ -42781,14 +42533,8 @@
       <c r="J90" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K90" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L90" t="s">
-        <v>1060</v>
-      </c>
       <c r="M90" s="159" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="N90" t="s">
         <v>1060</v>
@@ -42840,14 +42586,8 @@
       <c r="J91" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K91" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L91" t="s">
-        <v>1060</v>
-      </c>
       <c r="M91" s="159" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="N91" t="s">
         <v>1060</v>
@@ -42899,14 +42639,8 @@
       <c r="J92" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K92" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L92" t="s">
-        <v>1060</v>
-      </c>
       <c r="M92" s="159" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="N92" t="s">
         <v>1060</v>
@@ -42958,23 +42692,17 @@
       <c r="J93" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K93" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L93" t="s">
-        <v>1060</v>
-      </c>
       <c r="M93" s="159" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="N93" t="s">
         <v>1060</v>
       </c>
       <c r="O93" t="s">
+        <v>1572</v>
+      </c>
+      <c r="P93" s="10" t="s">
         <v>1573</v>
-      </c>
-      <c r="P93" s="10" t="s">
-        <v>1574</v>
       </c>
       <c r="Q93" s="10" t="s">
         <v>51</v>
@@ -43017,23 +42745,17 @@
       <c r="J94" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K94" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L94" t="s">
-        <v>1060</v>
-      </c>
       <c r="M94" s="159" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="N94" t="s">
         <v>1060</v>
       </c>
       <c r="O94" t="s">
+        <v>1575</v>
+      </c>
+      <c r="P94" s="10" t="s">
         <v>1576</v>
-      </c>
-      <c r="P94" s="10" t="s">
-        <v>1577</v>
       </c>
       <c r="Q94" s="10" t="s">
         <v>51</v>
@@ -43076,14 +42798,8 @@
       <c r="J95" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K95" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L95" t="s">
-        <v>1060</v>
-      </c>
       <c r="M95" s="159" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="N95" t="s">
         <v>1060</v>
@@ -43135,14 +42851,8 @@
       <c r="J96" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K96" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L96" t="s">
-        <v>1060</v>
-      </c>
       <c r="M96" s="159" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="N96" t="s">
         <v>1060</v>
@@ -43194,14 +42904,8 @@
       <c r="J97" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K97" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L97" t="s">
-        <v>1060</v>
-      </c>
       <c r="M97" s="159" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="N97" t="s">
         <v>1060</v>
@@ -43253,14 +42957,8 @@
       <c r="J98" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K98" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L98" t="s">
-        <v>1060</v>
-      </c>
       <c r="M98" s="159" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="N98" t="s">
         <v>1060</v>
@@ -43312,14 +43010,8 @@
       <c r="J99" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K99" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L99" t="s">
-        <v>1060</v>
-      </c>
       <c r="M99" s="159" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="N99" t="s">
         <v>1060</v>
@@ -43371,14 +43063,8 @@
       <c r="J100" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K100" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L100" t="s">
-        <v>1060</v>
-      </c>
       <c r="M100" s="159" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="N100" t="s">
         <v>1060</v>
@@ -43430,14 +43116,8 @@
       <c r="J101" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K101" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L101" t="s">
-        <v>1060</v>
-      </c>
       <c r="M101" s="159" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="N101" t="s">
         <v>1060</v>
@@ -43489,14 +43169,8 @@
       <c r="J102" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K102" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L102" t="s">
-        <v>1060</v>
-      </c>
       <c r="M102" s="159" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="N102" t="s">
         <v>1060</v>
@@ -43548,14 +43222,8 @@
       <c r="J103" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K103" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L103" t="s">
-        <v>1060</v>
-      </c>
       <c r="M103" s="159" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="N103" t="s">
         <v>1060</v>
@@ -43607,14 +43275,8 @@
       <c r="J104" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K104" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L104" t="s">
-        <v>1060</v>
-      </c>
       <c r="M104" s="159" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="N104" t="s">
         <v>1060</v>
@@ -43666,23 +43328,17 @@
       <c r="J105" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K105" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L105" t="s">
-        <v>1060</v>
-      </c>
       <c r="M105" s="159" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="N105" t="s">
         <v>1060</v>
       </c>
       <c r="O105" t="s">
+        <v>1588</v>
+      </c>
+      <c r="P105" s="10" t="s">
         <v>1589</v>
-      </c>
-      <c r="P105" s="10" t="s">
-        <v>1590</v>
       </c>
       <c r="Q105" s="10" t="s">
         <v>51</v>
@@ -43725,23 +43381,17 @@
       <c r="J106" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K106" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L106" t="s">
-        <v>1060</v>
-      </c>
       <c r="M106" s="159" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="N106" t="s">
         <v>1060</v>
       </c>
       <c r="O106" t="s">
+        <v>1591</v>
+      </c>
+      <c r="P106" s="10" t="s">
         <v>1592</v>
-      </c>
-      <c r="P106" s="10" t="s">
-        <v>1593</v>
       </c>
       <c r="Q106" s="10" t="s">
         <v>51</v>
@@ -43784,14 +43434,8 @@
       <c r="J107" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K107" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L107" t="s">
-        <v>1060</v>
-      </c>
       <c r="M107" s="159" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="N107" t="s">
         <v>1060</v>
@@ -43817,7 +43461,7 @@
         <v>1409</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="C108" s="10">
         <v>2</v>
@@ -43843,14 +43487,8 @@
       <c r="J108" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K108" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L108" t="s">
-        <v>1060</v>
-      </c>
       <c r="M108" s="159" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="N108" t="s">
         <v>1060</v>
@@ -43902,14 +43540,8 @@
       <c r="J109" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K109" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L109" t="s">
-        <v>1060</v>
-      </c>
       <c r="M109" s="159" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="N109" t="s">
         <v>1060</v>
@@ -43961,14 +43593,8 @@
       <c r="J110" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K110" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L110" t="s">
-        <v>1060</v>
-      </c>
       <c r="M110" s="159" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="N110" t="s">
         <v>1060</v>
@@ -44020,14 +43646,8 @@
       <c r="J111" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K111" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L111" t="s">
-        <v>1060</v>
-      </c>
       <c r="M111" s="159" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="N111" t="s">
         <v>1060</v>
@@ -44079,14 +43699,8 @@
       <c r="J112" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K112" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L112" t="s">
-        <v>1060</v>
-      </c>
       <c r="M112" s="159" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="N112" t="s">
         <v>1060</v>
@@ -44138,14 +43752,8 @@
       <c r="J113" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K113" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L113" t="s">
-        <v>1060</v>
-      </c>
       <c r="M113" s="159" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="N113" t="s">
         <v>1060</v>
@@ -44197,14 +43805,8 @@
       <c r="J114" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K114" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L114" t="s">
-        <v>1060</v>
-      </c>
       <c r="M114" s="159" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="N114" t="s">
         <v>1060</v>
@@ -44256,14 +43858,8 @@
       <c r="J115" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K115" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L115" t="s">
-        <v>1060</v>
-      </c>
       <c r="M115" s="159" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="N115" t="s">
         <v>1060</v>
@@ -44315,14 +43911,8 @@
       <c r="J116" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K116" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L116" t="s">
-        <v>1060</v>
-      </c>
       <c r="M116" s="159" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="N116" t="s">
         <v>1060</v>
@@ -44531,7 +44121,7 @@
     </row>
     <row r="2" spans="1:17" s="24" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -44610,10 +44200,10 @@
         <v>1221</v>
       </c>
       <c r="J7" s="45" t="s">
+        <v>1605</v>
+      </c>
+      <c r="K7" s="45" t="s">
         <v>1606</v>
-      </c>
-      <c r="K7" s="45" t="s">
-        <v>1607</v>
       </c>
       <c r="L7" s="54" t="s">
         <v>1224</v>
@@ -46246,7 +45836,7 @@
         <v>1165</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -46269,7 +45859,7 @@
         <v>1165</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -46292,7 +45882,7 @@
         <v>1165</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -46315,7 +45905,7 @@
         <v>1165</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -46338,7 +45928,7 @@
         <v>1165</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -46361,7 +45951,7 @@
         <v>1165</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -46439,7 +46029,7 @@
         <v>1165</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -46465,7 +46055,7 @@
         <v>1182</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -46491,7 +46081,7 @@
         <v>1165</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -46517,7 +46107,7 @@
         <v>1182</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -46543,7 +46133,7 @@
         <v>1165</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -46569,7 +46159,7 @@
         <v>1182</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -46595,7 +46185,7 @@
         <v>1165</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -46621,7 +46211,7 @@
         <v>1182</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -46644,7 +46234,7 @@
         <v>1165</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -46667,7 +46257,7 @@
         <v>1165</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -46693,7 +46283,7 @@
         <v>1182</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -46719,7 +46309,7 @@
         <v>1165</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -46771,7 +46361,7 @@
         <v>1165</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -46797,7 +46387,7 @@
         <v>1182</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -46901,7 +46491,7 @@
         <v>1165</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -46927,7 +46517,7 @@
         <v>1165</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -46950,7 +46540,7 @@
         <v>1165</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -47002,7 +46592,7 @@
         <v>1165</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -47025,7 +46615,7 @@
         <v>1165</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Address issues when iLO is in a managed state
</commit_message>
<xml_diff>
--- a/Example-Export-OV-sheets.xlsx
+++ b/Example-Export-OV-sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github-Temp\Import-Export-OneView-Resources-11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Repos\Import-Export-OneView-Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1090BA33-F3B2-409D-ADA7-D137985E4274}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57018D76-488B-4854-A484-7799229D8537}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="723" firstSheet="29" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="723" firstSheet="29" activeTab="35" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="11" r:id="rId1"/>
@@ -66,7 +66,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -74,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8152" uniqueCount="1633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8152" uniqueCount="1632">
   <si>
     <t>Pod</t>
   </si>
@@ -5923,9 +5922,6 @@
   </si>
   <si>
     <t>manageLocalStorage</t>
-  </si>
-  <si>
-    <t>manageMp</t>
   </si>
   <si>
     <t>iscsiInitiatorName</t>
@@ -7195,7 +7191,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -7648,9 +7644,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7664,6 +7657,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -8691,7 +8690,7 @@
         <v>185</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -8735,7 +8734,7 @@
         <v>187</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -8916,15 +8915,15 @@
       <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D14" s="170"/>
-      <c r="E14" s="170"/>
-      <c r="F14" s="170"/>
-      <c r="G14" s="170"/>
-      <c r="H14" s="170"/>
-      <c r="I14" s="170"/>
-      <c r="J14" s="170"/>
-      <c r="K14" s="170"/>
-      <c r="L14" s="170"/>
+      <c r="D14" s="175"/>
+      <c r="E14" s="175"/>
+      <c r="F14" s="175"/>
+      <c r="G14" s="175"/>
+      <c r="H14" s="175"/>
+      <c r="I14" s="175"/>
+      <c r="J14" s="175"/>
+      <c r="K14" s="175"/>
+      <c r="L14" s="175"/>
     </row>
     <row r="15" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
@@ -9046,7 +9045,7 @@
         <v>190</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C20" s="63" t="s">
         <v>51</v>
@@ -9069,7 +9068,7 @@
         <v>190</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="C21" s="63" t="s">
         <v>51</v>
@@ -9625,11 +9624,11 @@
       <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H14" s="170"/>
-      <c r="I14" s="170"/>
-      <c r="J14" s="170"/>
-      <c r="K14" s="170"/>
-      <c r="L14" s="170"/>
+      <c r="H14" s="175"/>
+      <c r="I14" s="175"/>
+      <c r="J14" s="175"/>
+      <c r="K14" s="175"/>
+      <c r="L14" s="175"/>
     </row>
     <row r="15" spans="1:12" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
@@ -9765,7 +9764,7 @@
         <v>164</v>
       </c>
       <c r="F21" s="63" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="G21" s="63" t="s">
         <v>249</v>
@@ -9788,7 +9787,7 @@
         <v>165</v>
       </c>
       <c r="F22" s="63" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="G22" s="63" t="s">
         <v>245</v>
@@ -16085,25 +16084,25 @@
       <c r="M13" s="23"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="D14" s="170"/>
-      <c r="E14" s="170"/>
-      <c r="F14" s="170"/>
-      <c r="G14" s="170"/>
-      <c r="H14" s="170"/>
-      <c r="I14" s="170"/>
-      <c r="J14" s="170"/>
-      <c r="K14" s="170"/>
-      <c r="L14" s="170"/>
-      <c r="M14" s="170"/>
-      <c r="N14" s="170"/>
-      <c r="O14" s="170"/>
-      <c r="P14" s="170"/>
-      <c r="Q14" s="170"/>
-      <c r="R14" s="170"/>
-      <c r="S14" s="170"/>
-      <c r="T14" s="170"/>
-      <c r="U14" s="170"/>
-      <c r="V14" s="170"/>
+      <c r="D14" s="175"/>
+      <c r="E14" s="175"/>
+      <c r="F14" s="175"/>
+      <c r="G14" s="175"/>
+      <c r="H14" s="175"/>
+      <c r="I14" s="175"/>
+      <c r="J14" s="175"/>
+      <c r="K14" s="175"/>
+      <c r="L14" s="175"/>
+      <c r="M14" s="175"/>
+      <c r="N14" s="175"/>
+      <c r="O14" s="175"/>
+      <c r="P14" s="175"/>
+      <c r="Q14" s="175"/>
+      <c r="R14" s="175"/>
+      <c r="S14" s="175"/>
+      <c r="T14" s="175"/>
+      <c r="U14" s="175"/>
+      <c r="V14" s="175"/>
     </row>
     <row r="15" spans="1:22" s="63" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="63" t="s">
@@ -16128,7 +16127,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="63" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="I15" s="63" t="s">
         <v>575</v>
@@ -16169,7 +16168,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="63" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="I16" s="157" t="s">
         <v>581</v>
@@ -16201,7 +16200,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="63" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="I17" s="157" t="s">
         <v>583</v>
@@ -16236,7 +16235,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="63" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="I18" s="63" t="s">
         <v>586</v>
@@ -16281,7 +16280,7 @@
         <v>0</v>
       </c>
       <c r="H19" s="63" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="I19" s="63" t="s">
         <v>588</v>
@@ -16323,7 +16322,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="63" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="I20" s="157" t="s">
         <v>590</v>
@@ -16362,7 +16361,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="63" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="I21" s="63" t="s">
         <v>591</v>
@@ -16394,7 +16393,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="63" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="I22" s="63" t="s">
         <v>592</v>
@@ -16426,7 +16425,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="63" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="I23" s="63" t="s">
         <v>591</v>
@@ -16458,7 +16457,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="63" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="I24" s="63" t="s">
         <v>592</v>
@@ -17968,7 +17967,7 @@
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="146" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="B15" s="146" t="s">
         <v>685</v>
@@ -22547,7 +22546,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="146" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="B39" s="146" t="s">
         <v>51</v>
@@ -22744,7 +22743,7 @@
     </row>
     <row r="15" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>864</v>
@@ -22853,13 +22852,13 @@
         <v>872</v>
       </c>
       <c r="D1" s="160" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>873</v>
       </c>
       <c r="F1" s="160" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="G1" s="153" t="s">
         <v>874</v>
@@ -22965,13 +22964,13 @@
         <v>883</v>
       </c>
       <c r="D7" s="164" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="E7" s="46" t="s">
         <v>884</v>
       </c>
       <c r="F7" s="164" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="G7" s="136" t="s">
         <v>885</v>
@@ -23076,7 +23075,7 @@
         <v>868</v>
       </c>
       <c r="F15" s="169" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>51</v>
@@ -25998,7 +25997,7 @@
     </row>
     <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>51</v>
@@ -26081,7 +26080,7 @@
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>51</v>
@@ -26176,7 +26175,7 @@
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>51</v>
@@ -29525,7 +29524,7 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>1190</v>
@@ -29569,7 +29568,7 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>1192</v>
@@ -29613,7 +29612,7 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>1193</v>
@@ -29657,7 +29656,7 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>1190</v>
@@ -29701,7 +29700,7 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>1192</v>
@@ -29745,7 +29744,7 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>1193</v>
@@ -32556,7 +32555,7 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>1234</v>
@@ -32591,7 +32590,7 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>1234</v>
@@ -32626,7 +32625,7 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>1234</v>
@@ -34863,7 +34862,7 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>1332</v>
@@ -34878,10 +34877,10 @@
         <v>103</v>
       </c>
       <c r="F15" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="G15" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="H15" t="s">
         <v>103</v>
@@ -34904,7 +34903,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B16" s="59" t="s">
         <v>1332</v>
@@ -34936,7 +34935,7 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B17" s="59" t="s">
         <v>1332</v>
@@ -34951,10 +34950,10 @@
         <v>103</v>
       </c>
       <c r="F17" t="s">
+        <v>1618</v>
+      </c>
+      <c r="G17" t="s">
         <v>1619</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1620</v>
       </c>
       <c r="H17" t="s">
         <v>103</v>
@@ -34977,7 +34976,7 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B18" s="59" t="s">
         <v>1332</v>
@@ -34992,10 +34991,10 @@
         <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="G18" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="H18" t="s">
         <v>103</v>
@@ -35018,7 +35017,7 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B19" s="59" t="s">
         <v>1332</v>
@@ -35080,7 +35079,7 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B20" s="59" t="s">
         <v>1332</v>
@@ -35121,7 +35120,7 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B21" s="59" t="s">
         <v>1332</v>
@@ -35162,7 +35161,7 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B22" s="59" t="s">
         <v>1332</v>
@@ -35203,7 +35202,7 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B23" s="59" t="s">
         <v>1332</v>
@@ -35238,7 +35237,7 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="B24" s="59" t="s">
         <v>1332</v>
@@ -35331,9 +35330,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -35366,7 +35365,7 @@
     <col min="34" max="34" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="11" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" s="11" customFormat="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>14</v>
       </c>
@@ -35442,8 +35441,8 @@
       <c r="Y1" s="109" t="s">
         <v>1014</v>
       </c>
-      <c r="Z1" s="109" t="s">
-        <v>1358</v>
+      <c r="Z1" s="176" t="s">
+        <v>1015</v>
       </c>
       <c r="AA1" s="11" t="s">
         <v>1017</v>
@@ -35461,7 +35460,7 @@
         <v>1020</v>
       </c>
       <c r="AF1" s="109" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="AG1" s="11" t="s">
         <v>1021</v>
@@ -35470,28 +35469,28 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:34" s="24" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" s="24" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
       <c r="E2" s="90"/>
     </row>
-    <row r="3" spans="1:34" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" s="22" customFormat="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>1023</v>
       </c>
       <c r="E3" s="90"/>
     </row>
-    <row r="4" spans="1:34" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" s="22" customFormat="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="90"/>
     </row>
-    <row r="5" spans="1:34" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" s="2" customFormat="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>434</v>
       </c>
@@ -35517,7 +35516,7 @@
       <c r="U5" s="27"/>
       <c r="V5" s="27"/>
     </row>
-    <row r="6" spans="1:34" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" s="2" customFormat="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26"/>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
@@ -35542,16 +35541,16 @@
       <c r="U6" s="23"/>
       <c r="V6" s="23"/>
     </row>
-    <row r="7" spans="1:34" s="15" customFormat="1" ht="380.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" s="15" customFormat="1" ht="380.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="48" t="s">
+        <v>1361</v>
+      </c>
+      <c r="D7" s="48" t="s">
         <v>1362</v>
-      </c>
-      <c r="D7" s="48" t="s">
-        <v>1363</v>
       </c>
       <c r="E7" s="92"/>
       <c r="F7" s="48" t="s">
@@ -35576,16 +35575,16 @@
         <v>1032</v>
       </c>
       <c r="M7" s="53" t="s">
+        <v>1363</v>
+      </c>
+      <c r="N7" s="53" t="s">
         <v>1364</v>
       </c>
-      <c r="N7" s="53" t="s">
+      <c r="O7" s="53" t="s">
         <v>1365</v>
       </c>
-      <c r="O7" s="53" t="s">
+      <c r="P7" s="53" t="s">
         <v>1366</v>
-      </c>
-      <c r="P7" s="53" t="s">
-        <v>1367</v>
       </c>
       <c r="Q7" s="54" t="s">
         <v>1037</v>
@@ -35603,7 +35602,7 @@
         <v>1041</v>
       </c>
       <c r="V7" s="46" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="W7" s="93" t="s">
         <v>1043</v>
@@ -35627,13 +35626,13 @@
         <v>1048</v>
       </c>
       <c r="AD7" s="93" t="s">
+        <v>1368</v>
+      </c>
+      <c r="AE7" s="93" t="s">
         <v>1369</v>
       </c>
-      <c r="AE7" s="93" t="s">
+      <c r="AF7" s="93" t="s">
         <v>1370</v>
-      </c>
-      <c r="AF7" s="93" t="s">
-        <v>1371</v>
       </c>
       <c r="AG7" s="93" t="s">
         <v>1050</v>
@@ -35642,7 +35641,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="8" spans="1:34" s="14" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" s="14" customFormat="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
@@ -35666,27 +35665,27 @@
       <c r="U8" s="15"/>
       <c r="V8" s="15"/>
     </row>
-    <row r="9" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E12" s="4"/>
       <c r="AH12" s="10"/>
     </row>
-    <row r="13" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E14" s="4"/>
       <c r="AH14" s="10"/>
     </row>
-    <row r="15" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>790</v>
       </c>
@@ -35758,13 +35757,13 @@
         <v>1061</v>
       </c>
       <c r="AF15" s="158" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="AG15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>942</v>
       </c>
@@ -35836,14 +35835,14 @@
         <v>1061</v>
       </c>
       <c r="AF16" s="158" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="AG16" t="b">
         <v>0</v>
       </c>
       <c r="AH16" s="10"/>
     </row>
-    <row r="17" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>988</v>
       </c>
@@ -35915,13 +35914,13 @@
         <v>1061</v>
       </c>
       <c r="AF17" s="158" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="AG17" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>717</v>
       </c>
@@ -35999,14 +35998,14 @@
         <v>1061</v>
       </c>
       <c r="AF18" s="158" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="AG18" t="b">
         <v>0</v>
       </c>
       <c r="AH18" s="10"/>
     </row>
-    <row r="19" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>726</v>
       </c>
@@ -36084,13 +36083,13 @@
         <v>1061</v>
       </c>
       <c r="AF19" s="158" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="AG19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>729</v>
       </c>
@@ -36168,14 +36167,14 @@
         <v>1061</v>
       </c>
       <c r="AF20" s="158" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="AG20" t="b">
         <v>0</v>
       </c>
       <c r="AH20" s="10"/>
     </row>
-    <row r="21" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>715</v>
       </c>
@@ -36253,13 +36252,13 @@
         <v>1061</v>
       </c>
       <c r="AF21" s="158" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="AG21" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>721</v>
       </c>
@@ -36337,14 +36336,14 @@
         <v>1061</v>
       </c>
       <c r="AF22" s="158" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="AG22" t="b">
         <v>0</v>
       </c>
       <c r="AH22" s="10"/>
     </row>
-    <row r="23" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>742</v>
       </c>
@@ -36422,13 +36421,13 @@
         <v>1061</v>
       </c>
       <c r="AF23" s="158" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="AG23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>736</v>
       </c>
@@ -36506,14 +36505,14 @@
         <v>1061</v>
       </c>
       <c r="AF24" s="158" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="AG24" t="b">
         <v>0</v>
       </c>
       <c r="AH24" s="10"/>
     </row>
-    <row r="25" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>723</v>
       </c>
@@ -36591,13 +36590,13 @@
         <v>1061</v>
       </c>
       <c r="AF25" s="158" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="AG25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>740</v>
       </c>
@@ -36675,14 +36674,14 @@
         <v>1061</v>
       </c>
       <c r="AF26" s="158" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="AG26" t="b">
         <v>0</v>
       </c>
       <c r="AH26" s="10"/>
     </row>
-    <row r="27" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>733</v>
       </c>
@@ -36759,13 +36758,13 @@
         <v>1061</v>
       </c>
       <c r="AF27" s="158" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="AG27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>731</v>
       </c>
@@ -36842,13 +36841,13 @@
         <v>1061</v>
       </c>
       <c r="AF28" s="158" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="AG28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>744</v>
       </c>
@@ -36925,13 +36924,13 @@
         <v>1061</v>
       </c>
       <c r="AF29" s="158" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="AG29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>707</v>
       </c>
@@ -37008,13 +37007,13 @@
         <v>1061</v>
       </c>
       <c r="AF30" s="158" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="AG30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>709</v>
       </c>
@@ -37091,13 +37090,13 @@
         <v>1061</v>
       </c>
       <c r="AF31" s="158" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="AG31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:34" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>971</v>
       </c>
@@ -37126,13 +37125,13 @@
         <v>155</v>
       </c>
       <c r="K32" s="10" t="s">
+        <v>1388</v>
+      </c>
+      <c r="L32" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="M32" s="59" t="s">
         <v>1389</v>
-      </c>
-      <c r="L32" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="M32" s="59" t="s">
-        <v>1390</v>
       </c>
       <c r="O32" s="10" t="b">
         <v>0</v>
@@ -37183,13 +37182,13 @@
         <v>1061</v>
       </c>
       <c r="AF32" s="158" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="AG32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>951</v>
       </c>
@@ -37218,13 +37217,13 @@
         <v>155</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="L33" s="10" t="b">
         <v>0</v>
       </c>
       <c r="M33" s="59" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="O33" s="10" t="b">
         <v>0</v>
@@ -37275,18 +37274,18 @@
         <v>1061</v>
       </c>
       <c r="AF33" s="158" t="s">
+        <v>1392</v>
+      </c>
+      <c r="AG33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
         <v>1393</v>
       </c>
-      <c r="AG33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:33" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>1394</v>
-      </c>
       <c r="B34" s="10" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="F34" s="10" t="s">
         <v>1064</v>
@@ -37343,24 +37342,24 @@
         <v>1060</v>
       </c>
       <c r="AD34" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="AE34" t="s">
         <v>1061</v>
       </c>
       <c r="AF34" s="158" t="s">
+        <v>1395</v>
+      </c>
+      <c r="AG34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
         <v>1396</v>
       </c>
-      <c r="AG34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:33" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="B35" s="10" t="s">
         <v>1397</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>1398</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>51</v>
@@ -37426,15 +37425,15 @@
         <v>1061</v>
       </c>
       <c r="AF35" s="158" t="s">
+        <v>1398</v>
+      </c>
+      <c r="AG35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
         <v>1399</v>
-      </c>
-      <c r="AG35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:33" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>1400</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>51</v>
@@ -37497,24 +37496,24 @@
         <v>1060</v>
       </c>
       <c r="AD36" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="AE36" t="s">
         <v>1061</v>
       </c>
       <c r="AF36" s="158" t="s">
+        <v>1401</v>
+      </c>
+      <c r="AG36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
         <v>1402</v>
       </c>
-      <c r="AG36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:33" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="B37" s="10" t="s">
         <v>1403</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>1404</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>1084</v>
@@ -37577,19 +37576,19 @@
         <v>1060</v>
       </c>
       <c r="AD37" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="AE37" t="s">
         <v>1061</v>
       </c>
       <c r="AF37" s="158" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="AG37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>796</v>
       </c>
@@ -37657,24 +37656,24 @@
         <v>1060</v>
       </c>
       <c r="AD38" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="AE38" t="s">
         <v>1061</v>
       </c>
       <c r="AF38" s="158" t="s">
+        <v>1407</v>
+      </c>
+      <c r="AG38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
         <v>1408</v>
       </c>
-      <c r="AG38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:33" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="B39" s="10" t="s">
         <v>1409</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>1410</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>1102</v>
@@ -37734,24 +37733,24 @@
         <v>1060</v>
       </c>
       <c r="AD39" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="AE39" t="s">
         <v>1061</v>
       </c>
       <c r="AF39" s="158" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="AG39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>787</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>1102</v>
@@ -37814,24 +37813,24 @@
         <v>1060</v>
       </c>
       <c r="AD40" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="AE40" t="s">
         <v>1061</v>
       </c>
       <c r="AF40" s="158" t="s">
+        <v>1414</v>
+      </c>
+      <c r="AG40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
         <v>1415</v>
       </c>
-      <c r="AG40" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:33" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+      <c r="B41" s="10" t="s">
         <v>1416</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>1417</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>1122</v>
@@ -37891,21 +37890,21 @@
         <v>1060</v>
       </c>
       <c r="AD41" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="AE41" t="s">
         <v>1061</v>
       </c>
       <c r="AF41" s="158" t="s">
+        <v>1418</v>
+      </c>
+      <c r="AG41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
         <v>1419</v>
-      </c>
-      <c r="AG41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:33" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>1420</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>51</v>
@@ -37965,21 +37964,21 @@
         <v>1060</v>
       </c>
       <c r="AD42" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="AE42" t="s">
         <v>1061</v>
       </c>
       <c r="AF42" s="158" t="s">
+        <v>1421</v>
+      </c>
+      <c r="AG42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
         <v>1422</v>
-      </c>
-      <c r="AG42" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:33" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>1423</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>51</v>
@@ -38030,19 +38029,19 @@
         <v>1060</v>
       </c>
       <c r="AD43" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="AE43" t="s">
         <v>1061</v>
       </c>
       <c r="AF43" s="158" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="AG43" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:33" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>427</v>
       </c>
@@ -38086,7 +38085,7 @@
         <v>1</v>
       </c>
       <c r="W44" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="X44" t="b">
         <v>0</v>
@@ -38104,13 +38103,13 @@
         <v>1060</v>
       </c>
       <c r="AD44" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="AE44" t="s">
         <v>1061</v>
       </c>
       <c r="AF44" s="158" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="AG44" t="b">
         <v>0</v>
@@ -38158,7 +38157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5476BCB0-492A-4349-9B4C-02D8DB45D26B}">
   <dimension ref="A1:T116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K1" sqref="K1:L1048576"/>
     </sheetView>
@@ -38216,11 +38215,11 @@
       <c r="J1" s="11" t="s">
         <v>1134</v>
       </c>
-      <c r="K1" s="171" t="s">
+      <c r="K1" s="170" t="s">
+        <v>1628</v>
+      </c>
+      <c r="L1" s="170" t="s">
         <v>1629</v>
-      </c>
-      <c r="L1" s="171" t="s">
-        <v>1630</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>1136</v>
@@ -38256,8 +38255,8 @@
       <c r="G2" s="38"/>
       <c r="I2" s="38"/>
       <c r="J2" s="38"/>
-      <c r="K2" s="172"/>
-      <c r="L2" s="172"/>
+      <c r="K2" s="171"/>
+      <c r="L2" s="171"/>
     </row>
     <row r="3" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
@@ -38267,8 +38266,8 @@
       <c r="G3" s="27"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
-      <c r="K3" s="173"/>
-      <c r="L3" s="173"/>
+      <c r="K3" s="172"/>
+      <c r="L3" s="172"/>
     </row>
     <row r="4" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
@@ -38278,8 +38277,8 @@
       <c r="G4" s="27"/>
       <c r="I4" s="27"/>
       <c r="J4" s="27"/>
-      <c r="K4" s="173"/>
-      <c r="L4" s="173"/>
+      <c r="K4" s="172"/>
+      <c r="L4" s="172"/>
     </row>
     <row r="5" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="61" t="s">
@@ -38289,8 +38288,8 @@
       <c r="G5" s="27"/>
       <c r="I5" s="27"/>
       <c r="J5" s="27"/>
-      <c r="K5" s="173"/>
-      <c r="L5" s="173"/>
+      <c r="K5" s="172"/>
+      <c r="L5" s="172"/>
     </row>
     <row r="6" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
@@ -38300,8 +38299,8 @@
       <c r="G6" s="27"/>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
-      <c r="K6" s="173"/>
-      <c r="L6" s="173"/>
+      <c r="K6" s="172"/>
+      <c r="L6" s="172"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
       <c r="S6" s="27"/>
@@ -38355,11 +38354,11 @@
       <c r="J8" s="54" t="s">
         <v>1155</v>
       </c>
-      <c r="K8" s="174" t="s">
+      <c r="K8" s="173" t="s">
+        <v>1630</v>
+      </c>
+      <c r="L8" s="173" t="s">
         <v>1631</v>
-      </c>
-      <c r="L8" s="174" t="s">
-        <v>1632</v>
       </c>
       <c r="M8" s="45" t="s">
         <v>1158</v>
@@ -38384,20 +38383,20 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K11" s="175"/>
-      <c r="L11" s="175"/>
+      <c r="K11" s="174"/>
+      <c r="L11" s="174"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K12" s="175"/>
-      <c r="L12" s="175"/>
+      <c r="K12" s="174"/>
+      <c r="L12" s="174"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K13" s="175"/>
-      <c r="L13" s="175"/>
+      <c r="K13" s="174"/>
+      <c r="L13" s="174"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="K14" s="175"/>
-      <c r="L14" s="175"/>
+      <c r="K14" s="174"/>
+      <c r="L14" s="174"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
@@ -38430,10 +38429,10 @@
       <c r="J15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="175"/>
-      <c r="L15" s="175"/>
+      <c r="K15" s="174"/>
+      <c r="L15" s="174"/>
       <c r="M15" s="159" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="N15" t="s">
         <v>1060</v>
@@ -38485,10 +38484,10 @@
       <c r="J16" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="175"/>
-      <c r="L16" s="175"/>
+      <c r="K16" s="174"/>
+      <c r="L16" s="174"/>
       <c r="M16" s="159" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="N16" t="s">
         <v>1060</v>
@@ -38540,19 +38539,19 @@
       <c r="J17" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="175"/>
-      <c r="L17" s="175"/>
+      <c r="K17" s="174"/>
+      <c r="L17" s="174"/>
       <c r="M17" s="159" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="N17" t="s">
         <v>1060</v>
       </c>
       <c r="O17" t="s">
+        <v>1431</v>
+      </c>
+      <c r="P17" s="10" t="s">
         <v>1432</v>
-      </c>
-      <c r="P17" s="10" t="s">
-        <v>1433</v>
       </c>
       <c r="Q17" s="10" t="s">
         <v>51</v>
@@ -38595,19 +38594,19 @@
       <c r="J18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K18" s="175"/>
-      <c r="L18" s="175"/>
+      <c r="K18" s="174"/>
+      <c r="L18" s="174"/>
       <c r="M18" s="159" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="N18" t="s">
         <v>1060</v>
       </c>
       <c r="O18" t="s">
+        <v>1434</v>
+      </c>
+      <c r="P18" s="10" t="s">
         <v>1435</v>
-      </c>
-      <c r="P18" s="10" t="s">
-        <v>1436</v>
       </c>
       <c r="Q18" s="10" t="s">
         <v>51</v>
@@ -38650,10 +38649,10 @@
       <c r="J19" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K19" s="175"/>
-      <c r="L19" s="175"/>
+      <c r="K19" s="174"/>
+      <c r="L19" s="174"/>
       <c r="M19" s="159" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="N19" t="s">
         <v>1060</v>
@@ -38705,10 +38704,10 @@
       <c r="J20" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K20" s="175"/>
-      <c r="L20" s="175"/>
+      <c r="K20" s="174"/>
+      <c r="L20" s="174"/>
       <c r="M20" s="159" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="N20" t="s">
         <v>1060</v>
@@ -38760,10 +38759,10 @@
       <c r="J21" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="175"/>
-      <c r="L21" s="175"/>
+      <c r="K21" s="174"/>
+      <c r="L21" s="174"/>
       <c r="M21" s="159" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="N21" t="s">
         <v>1060</v>
@@ -38815,10 +38814,10 @@
       <c r="J22" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K22" s="175"/>
-      <c r="L22" s="175"/>
+      <c r="K22" s="174"/>
+      <c r="L22" s="174"/>
       <c r="M22" s="159" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="N22" t="s">
         <v>1060</v>
@@ -38870,10 +38869,10 @@
       <c r="J23" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K23" s="175"/>
-      <c r="L23" s="175"/>
+      <c r="K23" s="174"/>
+      <c r="L23" s="174"/>
       <c r="M23" s="159" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="N23" t="s">
         <v>1060</v>
@@ -38925,10 +38924,10 @@
       <c r="J24" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K24" s="175"/>
-      <c r="L24" s="175"/>
+      <c r="K24" s="174"/>
+      <c r="L24" s="174"/>
       <c r="M24" s="159" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="N24" t="s">
         <v>1060</v>
@@ -38980,19 +38979,19 @@
       <c r="J25" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K25" s="175"/>
-      <c r="L25" s="175"/>
+      <c r="K25" s="174"/>
+      <c r="L25" s="174"/>
       <c r="M25" s="159" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="N25" t="s">
         <v>1060</v>
       </c>
       <c r="O25" t="s">
+        <v>1443</v>
+      </c>
+      <c r="P25" s="10" t="s">
         <v>1444</v>
-      </c>
-      <c r="P25" s="10" t="s">
-        <v>1445</v>
       </c>
       <c r="Q25" s="10" t="s">
         <v>51</v>
@@ -39035,19 +39034,19 @@
       <c r="J26" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K26" s="175"/>
-      <c r="L26" s="175"/>
+      <c r="K26" s="174"/>
+      <c r="L26" s="174"/>
       <c r="M26" s="159" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="N26" t="s">
         <v>1060</v>
       </c>
       <c r="O26" t="s">
+        <v>1446</v>
+      </c>
+      <c r="P26" s="10" t="s">
         <v>1447</v>
-      </c>
-      <c r="P26" s="10" t="s">
-        <v>1448</v>
       </c>
       <c r="Q26" s="10" t="s">
         <v>51</v>
@@ -39090,10 +39089,10 @@
       <c r="J27" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K27" s="175"/>
-      <c r="L27" s="175"/>
+      <c r="K27" s="174"/>
+      <c r="L27" s="174"/>
       <c r="M27" s="159" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="N27" t="s">
         <v>1060</v>
@@ -39145,10 +39144,10 @@
       <c r="J28" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K28" s="175"/>
-      <c r="L28" s="175"/>
+      <c r="K28" s="174"/>
+      <c r="L28" s="174"/>
       <c r="M28" s="159" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="N28" t="s">
         <v>1060</v>
@@ -39200,19 +39199,19 @@
       <c r="J29" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K29" s="175"/>
-      <c r="L29" s="175"/>
+      <c r="K29" s="174"/>
+      <c r="L29" s="174"/>
       <c r="M29" s="159" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="N29" t="s">
         <v>1060</v>
       </c>
       <c r="O29" t="s">
+        <v>1451</v>
+      </c>
+      <c r="P29" s="10" t="s">
         <v>1452</v>
-      </c>
-      <c r="P29" s="10" t="s">
-        <v>1453</v>
       </c>
       <c r="Q29" s="10" t="s">
         <v>51</v>
@@ -39255,19 +39254,19 @@
       <c r="J30" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K30" s="175"/>
-      <c r="L30" s="175"/>
+      <c r="K30" s="174"/>
+      <c r="L30" s="174"/>
       <c r="M30" s="159" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="N30" t="s">
         <v>1060</v>
       </c>
       <c r="O30" t="s">
+        <v>1454</v>
+      </c>
+      <c r="P30" s="10" t="s">
         <v>1455</v>
-      </c>
-      <c r="P30" s="10" t="s">
-        <v>1456</v>
       </c>
       <c r="Q30" s="10" t="s">
         <v>51</v>
@@ -39310,10 +39309,10 @@
       <c r="J31" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K31" s="175"/>
-      <c r="L31" s="175"/>
+      <c r="K31" s="174"/>
+      <c r="L31" s="174"/>
       <c r="M31" s="159" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="N31" t="s">
         <v>1060</v>
@@ -39365,10 +39364,10 @@
       <c r="J32" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K32" s="175"/>
-      <c r="L32" s="175"/>
+      <c r="K32" s="174"/>
+      <c r="L32" s="174"/>
       <c r="M32" s="159" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="N32" t="s">
         <v>1060</v>
@@ -39420,19 +39419,19 @@
       <c r="J33" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K33" s="175"/>
-      <c r="L33" s="175"/>
+      <c r="K33" s="174"/>
+      <c r="L33" s="174"/>
       <c r="M33" s="159" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="N33" t="s">
         <v>1060</v>
       </c>
       <c r="O33" t="s">
+        <v>1459</v>
+      </c>
+      <c r="P33" s="10" t="s">
         <v>1460</v>
-      </c>
-      <c r="P33" s="10" t="s">
-        <v>1461</v>
       </c>
       <c r="Q33" s="10" t="s">
         <v>51</v>
@@ -39475,19 +39474,19 @@
       <c r="J34" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K34" s="175"/>
-      <c r="L34" s="175"/>
+      <c r="K34" s="174"/>
+      <c r="L34" s="174"/>
       <c r="M34" s="159" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="N34" t="s">
         <v>1060</v>
       </c>
       <c r="O34" t="s">
+        <v>1462</v>
+      </c>
+      <c r="P34" s="10" t="s">
         <v>1463</v>
-      </c>
-      <c r="P34" s="10" t="s">
-        <v>1464</v>
       </c>
       <c r="Q34" s="10" t="s">
         <v>51</v>
@@ -39530,10 +39529,10 @@
       <c r="J35" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="175"/>
-      <c r="L35" s="175"/>
+      <c r="K35" s="174"/>
+      <c r="L35" s="174"/>
       <c r="M35" s="159" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="N35" t="s">
         <v>1060</v>
@@ -39585,10 +39584,10 @@
       <c r="J36" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K36" s="175"/>
-      <c r="L36" s="175"/>
+      <c r="K36" s="174"/>
+      <c r="L36" s="174"/>
       <c r="M36" s="159" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="N36" t="s">
         <v>1060</v>
@@ -39640,19 +39639,19 @@
       <c r="J37" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K37" s="175"/>
-      <c r="L37" s="175"/>
+      <c r="K37" s="174"/>
+      <c r="L37" s="174"/>
       <c r="M37" s="159" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="N37" t="s">
         <v>1060</v>
       </c>
       <c r="O37" t="s">
+        <v>1467</v>
+      </c>
+      <c r="P37" s="10" t="s">
         <v>1468</v>
-      </c>
-      <c r="P37" s="10" t="s">
-        <v>1469</v>
       </c>
       <c r="Q37" s="10" t="s">
         <v>51</v>
@@ -39695,19 +39694,19 @@
       <c r="J38" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K38" s="175"/>
-      <c r="L38" s="175"/>
+      <c r="K38" s="174"/>
+      <c r="L38" s="174"/>
       <c r="M38" s="159" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="N38" t="s">
         <v>1060</v>
       </c>
       <c r="O38" t="s">
+        <v>1470</v>
+      </c>
+      <c r="P38" s="10" t="s">
         <v>1471</v>
-      </c>
-      <c r="P38" s="10" t="s">
-        <v>1472</v>
       </c>
       <c r="Q38" s="10" t="s">
         <v>51</v>
@@ -39750,10 +39749,10 @@
       <c r="J39" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K39" s="175"/>
-      <c r="L39" s="175"/>
+      <c r="K39" s="174"/>
+      <c r="L39" s="174"/>
       <c r="M39" s="159" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="N39" t="s">
         <v>1060</v>
@@ -39805,10 +39804,10 @@
       <c r="J40" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K40" s="175"/>
-      <c r="L40" s="175"/>
+      <c r="K40" s="174"/>
+      <c r="L40" s="174"/>
       <c r="M40" s="159" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="N40" t="s">
         <v>1060</v>
@@ -39860,19 +39859,19 @@
       <c r="J41" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K41" s="175"/>
-      <c r="L41" s="175"/>
+      <c r="K41" s="174"/>
+      <c r="L41" s="174"/>
       <c r="M41" s="159" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="N41" t="s">
         <v>1060</v>
       </c>
       <c r="O41" t="s">
+        <v>1475</v>
+      </c>
+      <c r="P41" s="10" t="s">
         <v>1476</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>1477</v>
       </c>
       <c r="Q41" s="10" t="s">
         <v>51</v>
@@ -39915,19 +39914,19 @@
       <c r="J42" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K42" s="175"/>
-      <c r="L42" s="175"/>
+      <c r="K42" s="174"/>
+      <c r="L42" s="174"/>
       <c r="M42" s="159" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="N42" t="s">
         <v>1060</v>
       </c>
       <c r="O42" t="s">
+        <v>1478</v>
+      </c>
+      <c r="P42" s="10" t="s">
         <v>1479</v>
-      </c>
-      <c r="P42" s="10" t="s">
-        <v>1480</v>
       </c>
       <c r="Q42" s="10" t="s">
         <v>51</v>
@@ -39970,10 +39969,10 @@
       <c r="J43" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K43" s="175"/>
-      <c r="L43" s="175"/>
+      <c r="K43" s="174"/>
+      <c r="L43" s="174"/>
       <c r="M43" s="159" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="N43" t="s">
         <v>1060</v>
@@ -40025,10 +40024,10 @@
       <c r="J44" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K44" s="175"/>
-      <c r="L44" s="175"/>
+      <c r="K44" s="174"/>
+      <c r="L44" s="174"/>
       <c r="M44" s="159" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="N44" t="s">
         <v>1060</v>
@@ -40080,19 +40079,19 @@
       <c r="J45" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K45" s="175"/>
-      <c r="L45" s="175"/>
+      <c r="K45" s="174"/>
+      <c r="L45" s="174"/>
       <c r="M45" s="159" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="N45" t="s">
         <v>1060</v>
       </c>
       <c r="O45" t="s">
+        <v>1483</v>
+      </c>
+      <c r="P45" s="10" t="s">
         <v>1484</v>
-      </c>
-      <c r="P45" s="10" t="s">
-        <v>1485</v>
       </c>
       <c r="Q45" s="10" t="s">
         <v>51</v>
@@ -40135,19 +40134,19 @@
       <c r="J46" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K46" s="175"/>
-      <c r="L46" s="175"/>
+      <c r="K46" s="174"/>
+      <c r="L46" s="174"/>
       <c r="M46" s="159" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="N46" t="s">
         <v>1060</v>
       </c>
       <c r="O46" t="s">
+        <v>1486</v>
+      </c>
+      <c r="P46" s="10" t="s">
         <v>1487</v>
-      </c>
-      <c r="P46" s="10" t="s">
-        <v>1488</v>
       </c>
       <c r="Q46" s="10" t="s">
         <v>51</v>
@@ -40190,10 +40189,10 @@
       <c r="J47" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K47" s="175"/>
-      <c r="L47" s="175"/>
+      <c r="K47" s="174"/>
+      <c r="L47" s="174"/>
       <c r="M47" s="159" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="N47" t="s">
         <v>1060</v>
@@ -40245,10 +40244,10 @@
       <c r="J48" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K48" s="175"/>
-      <c r="L48" s="175"/>
+      <c r="K48" s="174"/>
+      <c r="L48" s="174"/>
       <c r="M48" s="159" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="N48" t="s">
         <v>1060</v>
@@ -40300,19 +40299,19 @@
       <c r="J49" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K49" s="175"/>
-      <c r="L49" s="175"/>
+      <c r="K49" s="174"/>
+      <c r="L49" s="174"/>
       <c r="M49" s="159" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="N49" t="s">
         <v>1060</v>
       </c>
       <c r="O49" t="s">
+        <v>1491</v>
+      </c>
+      <c r="P49" s="10" t="s">
         <v>1492</v>
-      </c>
-      <c r="P49" s="10" t="s">
-        <v>1493</v>
       </c>
       <c r="Q49" s="10" t="s">
         <v>51</v>
@@ -40355,19 +40354,19 @@
       <c r="J50" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K50" s="175"/>
-      <c r="L50" s="175"/>
+      <c r="K50" s="174"/>
+      <c r="L50" s="174"/>
       <c r="M50" s="159" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="N50" t="s">
         <v>1060</v>
       </c>
       <c r="O50" t="s">
+        <v>1494</v>
+      </c>
+      <c r="P50" s="10" t="s">
         <v>1495</v>
-      </c>
-      <c r="P50" s="10" t="s">
-        <v>1496</v>
       </c>
       <c r="Q50" s="10" t="s">
         <v>51</v>
@@ -40410,10 +40409,10 @@
       <c r="J51" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K51" s="175"/>
-      <c r="L51" s="175"/>
+      <c r="K51" s="174"/>
+      <c r="L51" s="174"/>
       <c r="M51" s="159" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="N51" t="s">
         <v>1060</v>
@@ -40465,10 +40464,10 @@
       <c r="J52" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K52" s="175"/>
-      <c r="L52" s="175"/>
+      <c r="K52" s="174"/>
+      <c r="L52" s="174"/>
       <c r="M52" s="159" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="N52" t="s">
         <v>1060</v>
@@ -40520,19 +40519,19 @@
       <c r="J53" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K53" s="175"/>
-      <c r="L53" s="175"/>
+      <c r="K53" s="174"/>
+      <c r="L53" s="174"/>
       <c r="M53" s="159" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="N53" t="s">
         <v>1060</v>
       </c>
       <c r="O53" t="s">
+        <v>1499</v>
+      </c>
+      <c r="P53" s="10" t="s">
         <v>1500</v>
-      </c>
-      <c r="P53" s="10" t="s">
-        <v>1501</v>
       </c>
       <c r="Q53" s="10" t="s">
         <v>51</v>
@@ -40575,19 +40574,19 @@
       <c r="J54" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K54" s="175"/>
-      <c r="L54" s="175"/>
+      <c r="K54" s="174"/>
+      <c r="L54" s="174"/>
       <c r="M54" s="159" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="N54" t="s">
         <v>1060</v>
       </c>
       <c r="O54" t="s">
+        <v>1502</v>
+      </c>
+      <c r="P54" s="10" t="s">
         <v>1503</v>
-      </c>
-      <c r="P54" s="10" t="s">
-        <v>1504</v>
       </c>
       <c r="Q54" s="10" t="s">
         <v>51</v>
@@ -40630,10 +40629,10 @@
       <c r="J55" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K55" s="175"/>
-      <c r="L55" s="175"/>
+      <c r="K55" s="174"/>
+      <c r="L55" s="174"/>
       <c r="M55" s="159" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="N55" t="s">
         <v>1060</v>
@@ -40685,10 +40684,10 @@
       <c r="J56" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K56" s="175"/>
-      <c r="L56" s="175"/>
+      <c r="K56" s="174"/>
+      <c r="L56" s="174"/>
       <c r="M56" s="159" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="N56" t="s">
         <v>1060</v>
@@ -40740,19 +40739,19 @@
       <c r="J57" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K57" s="175"/>
-      <c r="L57" s="175"/>
+      <c r="K57" s="174"/>
+      <c r="L57" s="174"/>
       <c r="M57" s="159" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="N57" t="s">
         <v>1060</v>
       </c>
       <c r="O57" t="s">
+        <v>1507</v>
+      </c>
+      <c r="P57" s="10" t="s">
         <v>1508</v>
-      </c>
-      <c r="P57" s="10" t="s">
-        <v>1509</v>
       </c>
       <c r="Q57" s="10" t="s">
         <v>51</v>
@@ -40795,19 +40794,19 @@
       <c r="J58" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K58" s="175"/>
-      <c r="L58" s="175"/>
+      <c r="K58" s="174"/>
+      <c r="L58" s="174"/>
       <c r="M58" s="159" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="N58" t="s">
         <v>1060</v>
       </c>
       <c r="O58" t="s">
+        <v>1510</v>
+      </c>
+      <c r="P58" s="10" t="s">
         <v>1511</v>
-      </c>
-      <c r="P58" s="10" t="s">
-        <v>1512</v>
       </c>
       <c r="Q58" s="10" t="s">
         <v>51</v>
@@ -40850,10 +40849,10 @@
       <c r="J59" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K59" s="175"/>
-      <c r="L59" s="175"/>
+      <c r="K59" s="174"/>
+      <c r="L59" s="174"/>
       <c r="M59" s="159" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="N59" t="s">
         <v>1060</v>
@@ -40905,10 +40904,10 @@
       <c r="J60" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K60" s="175"/>
-      <c r="L60" s="175"/>
+      <c r="K60" s="174"/>
+      <c r="L60" s="174"/>
       <c r="M60" s="159" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="N60" t="s">
         <v>1060</v>
@@ -40960,19 +40959,19 @@
       <c r="J61" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K61" s="175"/>
-      <c r="L61" s="175"/>
+      <c r="K61" s="174"/>
+      <c r="L61" s="174"/>
       <c r="M61" s="159" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="N61" t="s">
         <v>1060</v>
       </c>
       <c r="O61" t="s">
+        <v>1515</v>
+      </c>
+      <c r="P61" s="10" t="s">
         <v>1516</v>
-      </c>
-      <c r="P61" s="10" t="s">
-        <v>1517</v>
       </c>
       <c r="Q61" s="10" t="s">
         <v>51</v>
@@ -41015,19 +41014,19 @@
       <c r="J62" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K62" s="175"/>
-      <c r="L62" s="175"/>
+      <c r="K62" s="174"/>
+      <c r="L62" s="174"/>
       <c r="M62" s="159" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="N62" t="s">
         <v>1060</v>
       </c>
       <c r="O62" t="s">
+        <v>1518</v>
+      </c>
+      <c r="P62" s="10" t="s">
         <v>1519</v>
-      </c>
-      <c r="P62" s="10" t="s">
-        <v>1520</v>
       </c>
       <c r="Q62" s="10" t="s">
         <v>51</v>
@@ -41070,10 +41069,10 @@
       <c r="J63" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K63" s="175"/>
-      <c r="L63" s="175"/>
+      <c r="K63" s="174"/>
+      <c r="L63" s="174"/>
       <c r="M63" s="159" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="N63" t="s">
         <v>1060</v>
@@ -41125,10 +41124,10 @@
       <c r="J64" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K64" s="175"/>
-      <c r="L64" s="175"/>
+      <c r="K64" s="174"/>
+      <c r="L64" s="174"/>
       <c r="M64" s="159" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="N64" t="s">
         <v>1060</v>
@@ -41180,19 +41179,19 @@
       <c r="J65" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K65" s="175"/>
-      <c r="L65" s="175"/>
+      <c r="K65" s="174"/>
+      <c r="L65" s="174"/>
       <c r="M65" s="159" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="N65" t="s">
         <v>1060</v>
       </c>
       <c r="O65" t="s">
+        <v>1523</v>
+      </c>
+      <c r="P65" s="10" t="s">
         <v>1524</v>
-      </c>
-      <c r="P65" s="10" t="s">
-        <v>1525</v>
       </c>
       <c r="Q65" s="10" t="s">
         <v>51</v>
@@ -41235,19 +41234,19 @@
       <c r="J66" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K66" s="175"/>
-      <c r="L66" s="175"/>
+      <c r="K66" s="174"/>
+      <c r="L66" s="174"/>
       <c r="M66" s="159" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="N66" t="s">
         <v>1060</v>
       </c>
       <c r="O66" t="s">
+        <v>1526</v>
+      </c>
+      <c r="P66" s="10" t="s">
         <v>1527</v>
-      </c>
-      <c r="P66" s="10" t="s">
-        <v>1528</v>
       </c>
       <c r="Q66" s="10" t="s">
         <v>51</v>
@@ -41290,10 +41289,10 @@
       <c r="J67" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K67" s="175"/>
-      <c r="L67" s="175"/>
+      <c r="K67" s="174"/>
+      <c r="L67" s="174"/>
       <c r="M67" s="159" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="N67" t="s">
         <v>1060</v>
@@ -41345,10 +41344,10 @@
       <c r="J68" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K68" s="175"/>
-      <c r="L68" s="175"/>
+      <c r="K68" s="174"/>
+      <c r="L68" s="174"/>
       <c r="M68" s="159" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="N68" t="s">
         <v>1060</v>
@@ -41400,19 +41399,19 @@
       <c r="J69" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K69" s="175"/>
-      <c r="L69" s="175"/>
+      <c r="K69" s="174"/>
+      <c r="L69" s="174"/>
       <c r="M69" s="159" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="N69" t="s">
         <v>1060</v>
       </c>
       <c r="O69" t="s">
+        <v>1531</v>
+      </c>
+      <c r="P69" s="10" t="s">
         <v>1532</v>
-      </c>
-      <c r="P69" s="10" t="s">
-        <v>1533</v>
       </c>
       <c r="Q69" s="10" t="s">
         <v>51</v>
@@ -41455,19 +41454,19 @@
       <c r="J70" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K70" s="175"/>
-      <c r="L70" s="175"/>
+      <c r="K70" s="174"/>
+      <c r="L70" s="174"/>
       <c r="M70" s="159" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="N70" t="s">
         <v>1060</v>
       </c>
       <c r="O70" t="s">
+        <v>1534</v>
+      </c>
+      <c r="P70" s="10" t="s">
         <v>1535</v>
-      </c>
-      <c r="P70" s="10" t="s">
-        <v>1536</v>
       </c>
       <c r="Q70" s="10" t="s">
         <v>51</v>
@@ -41510,10 +41509,10 @@
       <c r="J71" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K71" s="175"/>
-      <c r="L71" s="175"/>
+      <c r="K71" s="174"/>
+      <c r="L71" s="174"/>
       <c r="M71" s="159" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="N71" t="s">
         <v>1060</v>
@@ -41565,10 +41564,10 @@
       <c r="J72" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K72" s="175"/>
-      <c r="L72" s="175"/>
+      <c r="K72" s="174"/>
+      <c r="L72" s="174"/>
       <c r="M72" s="159" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="N72" t="s">
         <v>1060</v>
@@ -41620,19 +41619,19 @@
       <c r="J73" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K73" s="175"/>
-      <c r="L73" s="175"/>
+      <c r="K73" s="174"/>
+      <c r="L73" s="174"/>
       <c r="M73" s="159" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="N73" t="s">
         <v>1060</v>
       </c>
       <c r="O73" t="s">
+        <v>1539</v>
+      </c>
+      <c r="P73" s="10" t="s">
         <v>1540</v>
-      </c>
-      <c r="P73" s="10" t="s">
-        <v>1541</v>
       </c>
       <c r="Q73" s="10" t="s">
         <v>51</v>
@@ -41675,19 +41674,19 @@
       <c r="J74" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K74" s="175"/>
-      <c r="L74" s="175"/>
+      <c r="K74" s="174"/>
+      <c r="L74" s="174"/>
       <c r="M74" s="159" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="N74" t="s">
         <v>1060</v>
       </c>
       <c r="O74" t="s">
+        <v>1542</v>
+      </c>
+      <c r="P74" s="10" t="s">
         <v>1543</v>
-      </c>
-      <c r="P74" s="10" t="s">
-        <v>1544</v>
       </c>
       <c r="Q74" s="10" t="s">
         <v>51</v>
@@ -41730,10 +41729,10 @@
       <c r="J75" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K75" s="175"/>
-      <c r="L75" s="175"/>
+      <c r="K75" s="174"/>
+      <c r="L75" s="174"/>
       <c r="M75" s="159" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="N75" t="s">
         <v>1060</v>
@@ -41785,10 +41784,10 @@
       <c r="J76" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="K76" s="175"/>
-      <c r="L76" s="175"/>
+      <c r="K76" s="174"/>
+      <c r="L76" s="174"/>
       <c r="M76" s="159" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="N76" t="s">
         <v>1060</v>
@@ -41840,19 +41839,19 @@
       <c r="J77" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K77" s="175"/>
-      <c r="L77" s="175"/>
+      <c r="K77" s="174"/>
+      <c r="L77" s="174"/>
       <c r="M77" s="159" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="N77" t="s">
         <v>1060</v>
       </c>
       <c r="O77" t="s">
+        <v>1547</v>
+      </c>
+      <c r="P77" s="10" t="s">
         <v>1548</v>
-      </c>
-      <c r="P77" s="10" t="s">
-        <v>1549</v>
       </c>
       <c r="Q77" s="10" t="s">
         <v>51</v>
@@ -41895,19 +41894,19 @@
       <c r="J78" s="10" t="s">
         <v>1183</v>
       </c>
-      <c r="K78" s="175"/>
-      <c r="L78" s="175"/>
+      <c r="K78" s="174"/>
+      <c r="L78" s="174"/>
       <c r="M78" s="159" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="N78" t="s">
         <v>1060</v>
       </c>
       <c r="O78" t="s">
+        <v>1550</v>
+      </c>
+      <c r="P78" s="10" t="s">
         <v>1551</v>
-      </c>
-      <c r="P78" s="10" t="s">
-        <v>1552</v>
       </c>
       <c r="Q78" s="10" t="s">
         <v>51</v>
@@ -41951,7 +41950,7 @@
         <v>51</v>
       </c>
       <c r="M79" s="159" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="N79" t="s">
         <v>1060</v>
@@ -42004,7 +42003,7 @@
         <v>51</v>
       </c>
       <c r="M80" s="159" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="N80" t="s">
         <v>1060</v>
@@ -42057,7 +42056,7 @@
         <v>51</v>
       </c>
       <c r="M81" s="159" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="N81" t="s">
         <v>1060</v>
@@ -42110,7 +42109,7 @@
         <v>51</v>
       </c>
       <c r="M82" s="159" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="N82" t="s">
         <v>1060</v>
@@ -42163,7 +42162,7 @@
         <v>51</v>
       </c>
       <c r="M83" s="159" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="N83" t="s">
         <v>1060</v>
@@ -42216,7 +42215,7 @@
         <v>51</v>
       </c>
       <c r="M84" s="159" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="N84" t="s">
         <v>1060</v>
@@ -42269,16 +42268,16 @@
         <v>51</v>
       </c>
       <c r="M85" s="159" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="N85" t="s">
         <v>1060</v>
       </c>
       <c r="O85" t="s">
+        <v>1559</v>
+      </c>
+      <c r="P85" s="10" t="s">
         <v>1560</v>
-      </c>
-      <c r="P85" s="10" t="s">
-        <v>1561</v>
       </c>
       <c r="Q85" s="10" t="s">
         <v>51</v>
@@ -42322,16 +42321,16 @@
         <v>51</v>
       </c>
       <c r="M86" s="159" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="N86" t="s">
         <v>1060</v>
       </c>
       <c r="O86" t="s">
+        <v>1562</v>
+      </c>
+      <c r="P86" s="10" t="s">
         <v>1563</v>
-      </c>
-      <c r="P86" s="10" t="s">
-        <v>1564</v>
       </c>
       <c r="Q86" s="10" t="s">
         <v>51</v>
@@ -42375,7 +42374,7 @@
         <v>51</v>
       </c>
       <c r="M87" s="159" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="N87" t="s">
         <v>1060</v>
@@ -42428,7 +42427,7 @@
         <v>51</v>
       </c>
       <c r="M88" s="159" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="N88" t="s">
         <v>1060</v>
@@ -42481,7 +42480,7 @@
         <v>51</v>
       </c>
       <c r="M89" s="159" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="N89" t="s">
         <v>1060</v>
@@ -42534,7 +42533,7 @@
         <v>51</v>
       </c>
       <c r="M90" s="159" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="N90" t="s">
         <v>1060</v>
@@ -42587,7 +42586,7 @@
         <v>51</v>
       </c>
       <c r="M91" s="159" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="N91" t="s">
         <v>1060</v>
@@ -42640,7 +42639,7 @@
         <v>51</v>
       </c>
       <c r="M92" s="159" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="N92" t="s">
         <v>1060</v>
@@ -42693,16 +42692,16 @@
         <v>51</v>
       </c>
       <c r="M93" s="159" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="N93" t="s">
         <v>1060</v>
       </c>
       <c r="O93" t="s">
+        <v>1571</v>
+      </c>
+      <c r="P93" s="10" t="s">
         <v>1572</v>
-      </c>
-      <c r="P93" s="10" t="s">
-        <v>1573</v>
       </c>
       <c r="Q93" s="10" t="s">
         <v>51</v>
@@ -42746,16 +42745,16 @@
         <v>51</v>
       </c>
       <c r="M94" s="159" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="N94" t="s">
         <v>1060</v>
       </c>
       <c r="O94" t="s">
+        <v>1574</v>
+      </c>
+      <c r="P94" s="10" t="s">
         <v>1575</v>
-      </c>
-      <c r="P94" s="10" t="s">
-        <v>1576</v>
       </c>
       <c r="Q94" s="10" t="s">
         <v>51</v>
@@ -42769,7 +42768,7 @@
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B95" s="10" t="s">
         <v>1186</v>
@@ -42799,7 +42798,7 @@
         <v>51</v>
       </c>
       <c r="M95" s="159" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="N95" t="s">
         <v>1060</v>
@@ -42822,7 +42821,7 @@
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B96" s="10" t="s">
         <v>1187</v>
@@ -42852,7 +42851,7 @@
         <v>51</v>
       </c>
       <c r="M96" s="159" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="N96" t="s">
         <v>1060</v>
@@ -42875,7 +42874,7 @@
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="B97" s="10" t="s">
         <v>1188</v>
@@ -42905,7 +42904,7 @@
         <v>51</v>
       </c>
       <c r="M97" s="159" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="N97" t="s">
         <v>1060</v>
@@ -42928,7 +42927,7 @@
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="B98" s="10" t="s">
         <v>1189</v>
@@ -42958,7 +42957,7 @@
         <v>51</v>
       </c>
       <c r="M98" s="159" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="N98" t="s">
         <v>1060</v>
@@ -43011,7 +43010,7 @@
         <v>51</v>
       </c>
       <c r="M99" s="159" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="N99" t="s">
         <v>1060</v>
@@ -43064,7 +43063,7 @@
         <v>51</v>
       </c>
       <c r="M100" s="159" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="N100" t="s">
         <v>1060</v>
@@ -43117,7 +43116,7 @@
         <v>51</v>
       </c>
       <c r="M101" s="159" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="N101" t="s">
         <v>1060</v>
@@ -43170,7 +43169,7 @@
         <v>51</v>
       </c>
       <c r="M102" s="159" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="N102" t="s">
         <v>1060</v>
@@ -43223,7 +43222,7 @@
         <v>51</v>
       </c>
       <c r="M103" s="159" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="N103" t="s">
         <v>1060</v>
@@ -43276,7 +43275,7 @@
         <v>51</v>
       </c>
       <c r="M104" s="159" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="N104" t="s">
         <v>1060</v>
@@ -43329,16 +43328,16 @@
         <v>51</v>
       </c>
       <c r="M105" s="159" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="N105" t="s">
         <v>1060</v>
       </c>
       <c r="O105" t="s">
+        <v>1587</v>
+      </c>
+      <c r="P105" s="10" t="s">
         <v>1588</v>
-      </c>
-      <c r="P105" s="10" t="s">
-        <v>1589</v>
       </c>
       <c r="Q105" s="10" t="s">
         <v>51</v>
@@ -43382,16 +43381,16 @@
         <v>51</v>
       </c>
       <c r="M106" s="159" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="N106" t="s">
         <v>1060</v>
       </c>
       <c r="O106" t="s">
+        <v>1590</v>
+      </c>
+      <c r="P106" s="10" t="s">
         <v>1591</v>
-      </c>
-      <c r="P106" s="10" t="s">
-        <v>1592</v>
       </c>
       <c r="Q106" s="10" t="s">
         <v>51</v>
@@ -43405,7 +43404,7 @@
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B107" s="10" t="s">
         <v>1196</v>
@@ -43435,7 +43434,7 @@
         <v>51</v>
       </c>
       <c r="M107" s="159" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="N107" t="s">
         <v>1060</v>
@@ -43458,10 +43457,10 @@
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="C108" s="10">
         <v>2</v>
@@ -43488,7 +43487,7 @@
         <v>51</v>
       </c>
       <c r="M108" s="159" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="N108" t="s">
         <v>1060</v>
@@ -43541,7 +43540,7 @@
         <v>51</v>
       </c>
       <c r="M109" s="159" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="N109" t="s">
         <v>1060</v>
@@ -43594,7 +43593,7 @@
         <v>51</v>
       </c>
       <c r="M110" s="159" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="N110" t="s">
         <v>1060</v>
@@ -43617,7 +43616,7 @@
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="B111" s="10" t="s">
         <v>1186</v>
@@ -43647,7 +43646,7 @@
         <v>51</v>
       </c>
       <c r="M111" s="159" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="N111" t="s">
         <v>1060</v>
@@ -43670,7 +43669,7 @@
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="B112" s="10" t="s">
         <v>1187</v>
@@ -43700,7 +43699,7 @@
         <v>51</v>
       </c>
       <c r="M112" s="159" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="N112" t="s">
         <v>1060</v>
@@ -43753,7 +43752,7 @@
         <v>51</v>
       </c>
       <c r="M113" s="159" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="N113" t="s">
         <v>1060</v>
@@ -43806,7 +43805,7 @@
         <v>51</v>
       </c>
       <c r="M114" s="159" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="N114" t="s">
         <v>1060</v>
@@ -43859,7 +43858,7 @@
         <v>51</v>
       </c>
       <c r="M115" s="159" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="N115" t="s">
         <v>1060</v>
@@ -43912,7 +43911,7 @@
         <v>51</v>
       </c>
       <c r="M116" s="159" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="N116" t="s">
         <v>1060</v>
@@ -44121,7 +44120,7 @@
     </row>
     <row r="2" spans="1:17" s="24" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -44200,10 +44199,10 @@
         <v>1221</v>
       </c>
       <c r="J7" s="45" t="s">
+        <v>1604</v>
+      </c>
+      <c r="K7" s="45" t="s">
         <v>1605</v>
-      </c>
-      <c r="K7" s="45" t="s">
-        <v>1606</v>
       </c>
       <c r="L7" s="54" t="s">
         <v>1224</v>
@@ -45836,7 +45835,7 @@
         <v>1165</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -45859,7 +45858,7 @@
         <v>1165</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -45882,7 +45881,7 @@
         <v>1165</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -45905,7 +45904,7 @@
         <v>1165</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -45928,7 +45927,7 @@
         <v>1165</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -45951,7 +45950,7 @@
         <v>1165</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -46029,7 +46028,7 @@
         <v>1165</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -46055,7 +46054,7 @@
         <v>1182</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -46081,7 +46080,7 @@
         <v>1165</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -46107,7 +46106,7 @@
         <v>1182</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -46133,7 +46132,7 @@
         <v>1165</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -46159,7 +46158,7 @@
         <v>1182</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -46185,7 +46184,7 @@
         <v>1165</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -46211,7 +46210,7 @@
         <v>1182</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -46234,7 +46233,7 @@
         <v>1165</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -46257,7 +46256,7 @@
         <v>1165</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -46283,7 +46282,7 @@
         <v>1182</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -46309,7 +46308,7 @@
         <v>1165</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -46361,7 +46360,7 @@
         <v>1165</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -46387,7 +46386,7 @@
         <v>1182</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -46491,7 +46490,7 @@
         <v>1165</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -46517,7 +46516,7 @@
         <v>1165</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -46540,7 +46539,7 @@
         <v>1165</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -46592,7 +46591,7 @@
         <v>1165</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -46615,7 +46614,7 @@
         <v>1165</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -47983,21 +47982,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008B306D734CEBD84FBBC41786449802E3" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="16005ef843dd214786fd86ac676497e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="54a4fa2c-6341-4596-b8d8-a2e023346efc" xmlns:ns4="f7c671b8-1a97-4c58-b6a9-b872d1c47c8e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2325c866b17d621340695414d4ca9b0e" ns3:_="" ns4:_="">
     <xsd:import namespace="54a4fa2c-6341-4596-b8d8-a2e023346efc"/>
@@ -48214,32 +48198,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43ECCFC7-29C2-4C1C-BA35-7A8B581B0FD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7c671b8-1a97-4c58-b6a9-b872d1c47c8e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="54a4fa2c-6341-4596-b8d8-a2e023346efc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08671FF-7385-4DFE-A0B1-F772E0CBF546}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7124AFE1-C9C5-46E7-A048-9DDD62293557}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -48256,4 +48230,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08671FF-7385-4DFE-A0B1-F772E0CBF546}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43ECCFC7-29C2-4C1C-BA35-7A8B581B0FD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f7c671b8-1a97-4c58-b6a9-b872d1c47c8e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="54a4fa2c-6341-4596-b8d8-a2e023346efc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>